<commit_message>
Tab to show data read from spreadsheet for debugging
Also added images of graphs of prognosis and conditional survival
</commit_message>
<xml_diff>
--- a/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
+++ b/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="conditions" sheetId="1" r:id="rId1"/>
@@ -546,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2609,7 +2609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Input selection made dynamic
</commit_message>
<xml_diff>
--- a/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
+++ b/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17920" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="conditions" sheetId="1" r:id="rId1"/>
@@ -30,17 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
-  <si>
-    <t>all</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="54">
   <si>
     <t>Ovarian cancer</t>
   </si>
   <si>
-    <t>CaOv</t>
-  </si>
-  <si>
     <t>DataSource</t>
   </si>
   <si>
@@ -65,24 +59,9 @@
     <t>ContributerURL</t>
   </si>
   <si>
-    <t>Synonyms</t>
-  </si>
-  <si>
-    <t>Abbr</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
-    <t>Outcome1</t>
-  </si>
-  <si>
-    <t>Outcome2</t>
-  </si>
-  <si>
-    <t>Death from all causes</t>
-  </si>
-  <si>
     <t>Disease-free survival</t>
   </si>
   <si>
@@ -116,9 +95,6 @@
     <t>AbstractURL</t>
   </si>
   <si>
-    <t>Cancer of the female genital tract or peritoneum</t>
-  </si>
-  <si>
     <t>Outcome</t>
   </si>
   <si>
@@ -192,6 +168,30 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>Melanoma</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Histology</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Extent</t>
+  </si>
+  <si>
+    <t>Co-morbidity</t>
   </si>
 </sst>
 </file>
@@ -544,198 +544,982 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="50.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2" t="e">
+        <f>CONCATENATE(#REF!, "_", E2, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q2" t="e">
+        <f>CONCATENATE(#REF!, "_", E2, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R2" t="e">
+        <f>CONCATENATE(#REF!, "_", E2, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S2" t="e">
+        <f>CONCATENATE(#REF!, "_", E2, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>10</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
+      <c r="P3" t="e">
+        <f>CONCATENATE(#REF!, "_", E3, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q3" t="e">
+        <f>CONCATENATE(#REF!, "_", E3, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R3" t="e">
+        <f>CONCATENATE(#REF!, "_", E3, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S3" t="e">
+        <f>CONCATENATE(#REF!, "_", E3, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f t="shared" ref="A4:A20" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4">
+        <v>10</v>
+      </c>
+      <c r="O4">
+        <v>10</v>
+      </c>
+      <c r="P4" t="e">
+        <f>CONCATENATE(#REF!, "_", E4, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q4" t="e">
+        <f>CONCATENATE(#REF!, "_", E4, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R4" t="e">
+        <f>CONCATENATE(#REF!, "_", E4, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S4" t="e">
+        <f>CONCATENATE(#REF!, "_", E4, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f>B3</f>
+        <v>Ovarian cancer</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5">
+        <v>10</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5" t="e">
+        <f>CONCATENATE(#REF!, "_", E5, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q5" t="e">
+        <f>CONCATENATE(#REF!, "_", E5, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R5" t="e">
+        <f>CONCATENATE(#REF!, "_", E5, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S5" t="e">
+        <f>CONCATENATE(#REF!, "_", E5, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6">
+        <v>10</v>
+      </c>
+      <c r="O6">
+        <v>10</v>
+      </c>
+      <c r="P6" t="e">
+        <f>CONCATENATE(#REF!, "_", E6, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q6" t="e">
+        <f>CONCATENATE(#REF!, "_", E6, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R6" t="e">
+        <f>CONCATENATE(#REF!, "_", E6, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S6" t="e">
+        <f>CONCATENATE(#REF!, "_", E6, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7">
+        <v>10</v>
+      </c>
+      <c r="O7">
+        <v>10</v>
+      </c>
+      <c r="P7" t="e">
+        <f>CONCATENATE(#REF!, "_", E7, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q7" t="e">
+        <f>CONCATENATE(#REF!, "_", E7, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R7" t="e">
+        <f>CONCATENATE(#REF!, "_", E7, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S7" t="e">
+        <f>CONCATENATE(#REF!, "_", E7, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f>B6</f>
+        <v>Ovarian cancer</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8">
+        <v>10</v>
+      </c>
+      <c r="O8">
+        <v>10</v>
+      </c>
+      <c r="P8" t="e">
+        <f>CONCATENATE(#REF!, "_", E8, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q8" t="e">
+        <f>CONCATENATE(#REF!, "_", E8, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R8" t="e">
+        <f>CONCATENATE(#REF!, "_", E8, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S8" t="e">
+        <f>CONCATENATE(#REF!, "_", E8, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="O9">
+        <v>10</v>
+      </c>
+      <c r="P9" t="e">
+        <f>CONCATENATE(#REF!, "_", E9, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q9" t="e">
+        <f>CONCATENATE(#REF!, "_", E9, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R9" t="e">
+        <f>CONCATENATE(#REF!, "_", E9, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S9" t="e">
+        <f>CONCATENATE(#REF!, "_", E9, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10">
+        <v>10</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+      <c r="P10" t="e">
+        <f>CONCATENATE(#REF!, "_", E10, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q10" t="e">
+        <f>CONCATENATE(#REF!, "_", E10, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R10" t="e">
+        <f>CONCATENATE(#REF!, "_", E10, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S10" t="e">
+        <f>CONCATENATE(#REF!, "_", E10, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <f>B9</f>
+        <v>Ovarian cancer</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11">
+        <v>10</v>
+      </c>
+      <c r="O11">
+        <v>10</v>
+      </c>
+      <c r="P11" t="e">
+        <f>CONCATENATE(#REF!, "_", E11, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q11" t="e">
+        <f>CONCATENATE(#REF!, "_", E11, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R11" t="e">
+        <f>CONCATENATE(#REF!, "_", E11, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S11" t="e">
+        <f>CONCATENATE(#REF!, "_", E11, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <v>10</v>
+      </c>
+      <c r="P12" t="e">
+        <f>CONCATENATE(#REF!, "_", E12, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q12" t="e">
+        <f>CONCATENATE(#REF!, "_", E12, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R12" t="e">
+        <f>CONCATENATE(#REF!, "_", E12, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S12" t="e">
+        <f>CONCATENATE(#REF!, "_", E12, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13">
+        <v>10</v>
+      </c>
+      <c r="O13">
+        <v>10</v>
+      </c>
+      <c r="P13" t="e">
+        <f>CONCATENATE(#REF!, "_", E13, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q13" t="e">
+        <f>CONCATENATE(#REF!, "_", E13, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R13" t="e">
+        <f>CONCATENATE(#REF!, "_", E13, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S13" t="e">
+        <f>CONCATENATE(#REF!, "_", E13, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <v>10</v>
+      </c>
+      <c r="O14">
+        <v>10</v>
+      </c>
+      <c r="P14" t="e">
+        <f>CONCATENATE(#REF!, "_", E14, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q14" t="e">
+        <f>CONCATENATE(#REF!, "_", E14, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R14" t="e">
+        <f>CONCATENATE(#REF!, "_", E14, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S14" t="e">
+        <f>CONCATENATE(#REF!, "_", E14, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15">
+        <v>10</v>
+      </c>
+      <c r="O15">
+        <v>10</v>
+      </c>
+      <c r="P15" t="e">
+        <f>CONCATENATE(#REF!, "_", E15, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q15" t="e">
+        <f>CONCATENATE(#REF!, "_", E15, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R15" t="e">
+        <f>CONCATENATE(#REF!, "_", E15, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S15" t="e">
+        <f>CONCATENATE(#REF!, "_", E15, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16">
+        <v>10</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="P16" t="e">
+        <f>CONCATENATE(#REF!, "_", E16, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q16" t="e">
+        <f>CONCATENATE(#REF!, "_", E16, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R16" t="e">
+        <f>CONCATENATE(#REF!, "_", E16, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S16" t="e">
+        <f>CONCATENATE(#REF!, "_", E16, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17">
+        <v>10</v>
+      </c>
+      <c r="O17">
+        <v>10</v>
+      </c>
+      <c r="P17" t="e">
+        <f>CONCATENATE(#REF!, "_", E17, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q17" t="e">
+        <f>CONCATENATE(#REF!, "_", E17, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R17" t="e">
+        <f>CONCATENATE(#REF!, "_", E17, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S17" t="e">
+        <f>CONCATENATE(#REF!, "_", E17, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O2">
-        <v>10</v>
-      </c>
-      <c r="P2">
-        <v>10</v>
-      </c>
-      <c r="Q2" t="str">
-        <f>CONCATENATE(C2, "_", E2, "_data.xlsx")</f>
-        <v>all_example_data.xlsx</v>
-      </c>
-      <c r="R2" t="str">
-        <f>CONCATENATE(C2, "_", E2, "_about.html")</f>
-        <v>all_example_about.html</v>
-      </c>
-      <c r="S2" t="str">
-        <f>CONCATENATE(C2, "_", E2, "_Fig_1.html")</f>
-        <v>all_example_Fig_1.html</v>
-      </c>
-      <c r="T2" t="str">
-        <f>CONCATENATE(C2, "_", E2, "_Fig_2.html")</f>
-        <v>all_example_Fig_2.html</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="M18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18">
+        <v>10</v>
+      </c>
+      <c r="O18">
+        <v>10</v>
+      </c>
+      <c r="P18" t="e">
+        <f>CONCATENATE(#REF!, "_", E18, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q18" t="e">
+        <f>CONCATENATE(#REF!, "_", E18, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R18" t="e">
+        <f>CONCATENATE(#REF!, "_", E18, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S18" t="e">
+        <f>CONCATENATE(#REF!, "_", E18, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O3">
-        <v>10</v>
-      </c>
-      <c r="P3">
-        <v>10</v>
-      </c>
-      <c r="Q3" t="str">
-        <f>CONCATENATE(C3, "_", E3, "_data.xlsx")</f>
-        <v>CaOv_SEER_1989-2006_data.xlsx</v>
-      </c>
-      <c r="R3" t="str">
-        <f>CONCATENATE(C3, "_", E3, "_about.html")</f>
-        <v>CaOv_SEER_1989-2006_about.html</v>
-      </c>
-      <c r="S3" t="str">
-        <f>CONCATENATE(C3, "_", E3, "_Fig_1.html")</f>
-        <v>CaOv_SEER_1989-2006_Fig_1.html</v>
-      </c>
-      <c r="T3" t="str">
-        <f>CONCATENATE(C3, "_", E3, "_Fig_2.html")</f>
-        <v>CaOv_SEER_1989-2006_Fig_2.html</v>
+      <c r="M19" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19">
+        <v>10</v>
+      </c>
+      <c r="O19">
+        <v>10</v>
+      </c>
+      <c r="P19" t="e">
+        <f>CONCATENATE(#REF!, "_", E19, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q19" t="e">
+        <f>CONCATENATE(#REF!, "_", E19, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R19" t="e">
+        <f>CONCATENATE(#REF!, "_", E19, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S19" t="e">
+        <f>CONCATENATE(#REF!, "_", E19, "_Fig_2.html")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20">
+        <v>10</v>
+      </c>
+      <c r="O20">
+        <v>10</v>
+      </c>
+      <c r="P20" t="e">
+        <f>CONCATENATE(#REF!, "_", E20, "_data.xlsx")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q20" t="e">
+        <f>CONCATENATE(#REF!, "_", E20, "_about.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R20" t="e">
+        <f>CONCATENATE(#REF!, "_", E20, "_Fig_1.html")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S20" t="e">
+        <f>CONCATENATE(#REF!, "_", E20, "_Fig_2.html")</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G6" r:id="rId4"/>
+    <hyperlink ref="G8" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G9" r:id="rId7"/>
+    <hyperlink ref="G11" r:id="rId8"/>
+    <hyperlink ref="G10" r:id="rId9"/>
+    <hyperlink ref="G12" r:id="rId10"/>
+    <hyperlink ref="G14" r:id="rId11"/>
+    <hyperlink ref="G13" r:id="rId12"/>
+    <hyperlink ref="G15" r:id="rId13"/>
+    <hyperlink ref="G17" r:id="rId14"/>
+    <hyperlink ref="G16" r:id="rId15"/>
+    <hyperlink ref="G18" r:id="rId16"/>
+    <hyperlink ref="G20" r:id="rId17"/>
+    <hyperlink ref="G19" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -765,40 +1549,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="K1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -808,17 +1592,17 @@
       </c>
       <c r="B2" s="4" t="str">
         <f>conditions!B2</f>
-        <v>all</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <f>conditions!M2</f>
-        <v>Death from all causes</v>
+        <v>Example</v>
+      </c>
+      <c r="C2" s="4" t="e">
+        <f>conditions!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
@@ -846,11 +1630,11 @@
       </c>
       <c r="B3" s="4" t="str">
         <f>B2</f>
-        <v>all</v>
-      </c>
-      <c r="C3" s="4" t="str">
+        <v>Example</v>
+      </c>
+      <c r="C3" s="4" t="e">
         <f>C2</f>
-        <v>Death from all causes</v>
+        <v>#REF!</v>
       </c>
       <c r="D3" s="4" t="str">
         <f>D2</f>
@@ -887,11 +1671,11 @@
       </c>
       <c r="B4" s="4" t="str">
         <f t="shared" ref="B4:B12" si="2">B3</f>
-        <v>all</v>
-      </c>
-      <c r="C4" s="4" t="str">
+        <v>Example</v>
+      </c>
+      <c r="C4" s="4" t="e">
         <f t="shared" ref="C4:C12" si="3">C3</f>
-        <v>Death from all causes</v>
+        <v>#REF!</v>
       </c>
       <c r="D4" s="4" t="str">
         <f t="shared" ref="D4:E12" si="4">D3</f>
@@ -928,11 +1712,11 @@
       </c>
       <c r="B5" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>all</v>
-      </c>
-      <c r="C5" s="4" t="str">
+        <v>Example</v>
+      </c>
+      <c r="C5" s="4" t="e">
         <f t="shared" si="3"/>
-        <v>Death from all causes</v>
+        <v>#REF!</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" si="4"/>
@@ -969,11 +1753,11 @@
       </c>
       <c r="B6" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>all</v>
-      </c>
-      <c r="C6" s="4" t="str">
+        <v>Example</v>
+      </c>
+      <c r="C6" s="4" t="e">
         <f t="shared" si="3"/>
-        <v>Death from all causes</v>
+        <v>#REF!</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="4"/>
@@ -1010,11 +1794,11 @@
       </c>
       <c r="B7" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>all</v>
-      </c>
-      <c r="C7" s="4" t="str">
+        <v>Example</v>
+      </c>
+      <c r="C7" s="4" t="e">
         <f t="shared" si="3"/>
-        <v>Death from all causes</v>
+        <v>#REF!</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="4"/>
@@ -1051,11 +1835,11 @@
       </c>
       <c r="B8" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>all</v>
-      </c>
-      <c r="C8" s="4" t="str">
+        <v>Example</v>
+      </c>
+      <c r="C8" s="4" t="e">
         <f t="shared" si="3"/>
-        <v>Death from all causes</v>
+        <v>#REF!</v>
       </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="4"/>
@@ -1083,11 +1867,11 @@
       </c>
       <c r="B9" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>all</v>
-      </c>
-      <c r="C9" s="4" t="str">
+        <v>Example</v>
+      </c>
+      <c r="C9" s="4" t="e">
         <f t="shared" si="3"/>
-        <v>Death from all causes</v>
+        <v>#REF!</v>
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="4"/>
@@ -1115,11 +1899,11 @@
       </c>
       <c r="B10" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>all</v>
-      </c>
-      <c r="C10" s="4" t="str">
+        <v>Example</v>
+      </c>
+      <c r="C10" s="4" t="e">
         <f t="shared" si="3"/>
-        <v>Death from all causes</v>
+        <v>#REF!</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="4"/>
@@ -1147,11 +1931,11 @@
       </c>
       <c r="B11" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>all</v>
-      </c>
-      <c r="C11" s="4" t="str">
+        <v>Example</v>
+      </c>
+      <c r="C11" s="4" t="e">
         <f t="shared" si="3"/>
-        <v>Death from all causes</v>
+        <v>#REF!</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="4"/>
@@ -1179,11 +1963,11 @@
       </c>
       <c r="B12" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>all</v>
-      </c>
-      <c r="C12" s="4" t="str">
+        <v>Example</v>
+      </c>
+      <c r="C12" s="4" t="e">
         <f t="shared" si="3"/>
-        <v>Death from all causes</v>
+        <v>#REF!</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="4"/>
@@ -1214,13 +1998,13 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F13" s="4">
         <v>0</v>
@@ -1555,21 +2339,21 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <f>conditions!A14</f>
-        <v>0</v>
-      </c>
-      <c r="B24" s="4">
-        <f>conditions!B14</f>
-        <v>0</v>
+        <f>conditions!A15</f>
+        <v>14</v>
+      </c>
+      <c r="B24" s="4" t="str">
+        <f>conditions!B15</f>
+        <v>Melanoma</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F24" s="4">
         <v>0</v>
@@ -1585,11 +2369,11 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <f>A24</f>
-        <v>0</v>
-      </c>
-      <c r="B25" s="4">
+        <v>14</v>
+      </c>
+      <c r="B25" s="4" t="str">
         <f>B24</f>
-        <v>0</v>
+        <v>Melanoma</v>
       </c>
       <c r="C25" s="4" t="str">
         <f>C24</f>
@@ -1617,11 +2401,11 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <f t="shared" ref="A26:E34" si="12">A25</f>
-        <v>0</v>
-      </c>
-      <c r="B26" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B26" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>Melanoma</v>
       </c>
       <c r="C26" s="4" t="str">
         <f t="shared" si="12"/>
@@ -1649,11 +2433,11 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="B27" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B27" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>Melanoma</v>
       </c>
       <c r="C27" s="4" t="str">
         <f t="shared" si="12"/>
@@ -1681,11 +2465,11 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="B28" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B28" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>Melanoma</v>
       </c>
       <c r="C28" s="4" t="str">
         <f t="shared" si="12"/>
@@ -1713,11 +2497,11 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="B29" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B29" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>Melanoma</v>
       </c>
       <c r="C29" s="4" t="str">
         <f t="shared" si="12"/>
@@ -1745,11 +2529,11 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="B30" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B30" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>Melanoma</v>
       </c>
       <c r="C30" s="4" t="str">
         <f t="shared" si="12"/>
@@ -1777,11 +2561,11 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="B31" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B31" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>Melanoma</v>
       </c>
       <c r="C31" s="4" t="str">
         <f t="shared" si="12"/>
@@ -1809,11 +2593,11 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="B32" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B32" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>Melanoma</v>
       </c>
       <c r="C32" s="4" t="str">
         <f t="shared" si="12"/>
@@ -1841,11 +2625,11 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="B33" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B33" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>Melanoma</v>
       </c>
       <c r="C33" s="4" t="str">
         <f t="shared" si="12"/>
@@ -1873,11 +2657,11 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="B34" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B34" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>Melanoma</v>
       </c>
       <c r="C34" s="4" t="str">
         <f t="shared" si="12"/>
@@ -1904,21 +2688,21 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
-        <f>conditions!A25</f>
+        <f>conditions!A26</f>
         <v>0</v>
       </c>
       <c r="B35" s="4">
-        <f>conditions!B25</f>
+        <f>conditions!B26</f>
         <v>0</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F35" s="4">
         <v>0</v>
@@ -2253,21 +3037,21 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
-        <f>conditions!A36</f>
+        <f>conditions!A37</f>
         <v>0</v>
       </c>
       <c r="B46" s="4">
-        <f>conditions!B36</f>
+        <f>conditions!B37</f>
         <v>0</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F46" s="4">
         <v>0</v>
@@ -2609,7 +3393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -2620,25 +3404,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2668,10 +3452,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pretty prognosis plot - unreactive
</commit_message>
<xml_diff>
--- a/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
+++ b/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="105">
   <si>
     <t>Ovarian cancer</t>
   </si>
@@ -151,9 +151,6 @@
     <t>ExampleCondition</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>Conditional survival</t>
   </si>
   <si>
@@ -163,21 +160,9 @@
     <t>CIUL</t>
   </si>
   <si>
-    <t>Group 1</t>
-  </si>
-  <si>
-    <t>Group 2</t>
-  </si>
-  <si>
     <t>Age group</t>
   </si>
   <si>
-    <t>Worst</t>
-  </si>
-  <si>
-    <t>Best</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -187,12 +172,6 @@
     <t>Michael Power</t>
   </si>
   <si>
-    <t>Group 1 name</t>
-  </si>
-  <si>
-    <t>Group 2 name</t>
-  </si>
-  <si>
     <t>Choi M, Fuller CD, Thomas CR Jr, Wang SJ. Conditional survival in ovarian cancer: results from the SEER dataset 1988-2001. Gynecol Oncol. 2008 May;109(2):203-9. doi: 10.1016/j.ygyno.2008.01.033. Epub 2008 Mar 7. PubMed PMID: 18329082.</t>
   </si>
   <si>
@@ -229,15 +208,9 @@
     <t>PlotName</t>
   </si>
   <si>
-    <t>X-lab</t>
-  </si>
-  <si>
     <t>years</t>
   </si>
   <si>
-    <t>Y-lab</t>
-  </si>
-  <si>
     <t>5-year relative proportion survival</t>
   </si>
   <si>
@@ -332,6 +305,51 @@
   </si>
   <si>
     <t>Ovarian cancer 5-yr conditional survival by age-group and stage</t>
+  </si>
+  <si>
+    <t>PlotID</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>Plot_Dataset</t>
+  </si>
+  <si>
+    <t>DatasetID</t>
+  </si>
+  <si>
+    <t>Group1</t>
+  </si>
+  <si>
+    <t>Group2</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>WBmax</t>
+  </si>
+  <si>
+    <t>WBmin</t>
+  </si>
+  <si>
+    <t>Ylab</t>
+  </si>
+  <si>
+    <t>Xlab</t>
+  </si>
+  <si>
+    <t>Group1Name</t>
+  </si>
+  <si>
+    <t>Group2Name</t>
   </si>
 </sst>
 </file>
@@ -403,7 +421,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -472,6 +490,12 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -752,409 +776,438 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M29" sqref="M29"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="16"/>
+    <col min="1" max="1" width="10.83203125" style="20"/>
     <col min="2" max="2" width="14.1640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="17" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.83203125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="17.83203125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="57.5" style="7" customWidth="1"/>
-    <col min="16" max="16" width="42.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" style="9"/>
-    <col min="19" max="16384" width="10.83203125" style="16"/>
+    <col min="3" max="3" width="6.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.33203125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="17" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.83203125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="17.83203125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="58.5" style="7" customWidth="1"/>
+    <col min="18" max="18" width="42.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" style="9"/>
+    <col min="21" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="6"/>
+    </row>
+    <row r="2" spans="1:20" s="17" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="17" t="str">
+        <f>CONCATENATE(D2," (",B2,")")</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="19"/>
+    </row>
+    <row r="3" spans="1:20" s="17" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="25">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="17" t="str">
+        <f t="shared" ref="E3:E4" si="0">CONCATENATE(D3," (",B3,")")</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="K3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="19"/>
+    </row>
+    <row r="4" spans="1:20" s="17" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="25">
+        <v>1</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="R1" s="6"/>
-    </row>
-    <row r="2" spans="1:18" s="17" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A2" s="17">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="J4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="L4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" s="18" t="s">
+      <c r="O4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="R2" s="19"/>
-    </row>
-    <row r="3" spans="1:18" s="17" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A3" s="17">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" s="19"/>
-    </row>
-    <row r="4" spans="1:18" s="17" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A4" s="17">
-        <v>1</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="S4" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="P4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q4" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="19"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="J7" s="11"/>
+      <c r="T4" s="19"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
       <c r="N7" s="11"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="J8" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
       <c r="N8" s="11"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="J9" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
       <c r="N9" s="11"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="J10" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
       <c r="N10" s="11"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="J11" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
       <c r="N11" s="11"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="J12" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
       <c r="N12" s="11"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="J13" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
       <c r="N13" s="11"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="J14" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
       <c r="N14" s="11"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
       <c r="Q16" s="11"/>
-      <c r="R16" s="10"/>
-    </row>
-    <row r="17" spans="5:18" x14ac:dyDescent="0.2">
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="10"/>
+    </row>
+    <row r="17" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
       <c r="Q17" s="11"/>
-      <c r="R17" s="10"/>
-    </row>
-    <row r="20" spans="5:18" x14ac:dyDescent="0.2">
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="10"/>
+    </row>
+    <row r="20" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
       <c r="Q20" s="11"/>
-      <c r="R20" s="10"/>
-    </row>
-    <row r="21" spans="5:18" x14ac:dyDescent="0.2">
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="10"/>
+    </row>
+    <row r="21" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
       <c r="Q21" s="11"/>
-      <c r="R21" s="10"/>
-    </row>
-    <row r="24" spans="5:18" x14ac:dyDescent="0.2">
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="10"/>
+    </row>
+    <row r="24" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
       <c r="Q24" s="11"/>
-      <c r="R24" s="10"/>
-    </row>
-    <row r="25" spans="5:18" x14ac:dyDescent="0.2">
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="10"/>
+    </row>
+    <row r="25" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
       <c r="Q25" s="11"/>
-      <c r="R25" s="10"/>
-    </row>
-    <row r="31" spans="5:18" x14ac:dyDescent="0.2">
-      <c r="K31" s="11"/>
-    </row>
-    <row r="32" spans="5:18" x14ac:dyDescent="0.2">
-      <c r="K32" s="11"/>
-    </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K33" s="11"/>
-    </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K34" s="11"/>
-    </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K35" s="11"/>
-    </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K36" s="11"/>
-    </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K37" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="10"/>
+    </row>
+    <row r="31" spans="7:20" x14ac:dyDescent="0.2">
+      <c r="M31" s="11"/>
+    </row>
+    <row r="32" spans="7:20" x14ac:dyDescent="0.2">
+      <c r="M32" s="11"/>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M33" s="11"/>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M34" s="11"/>
+    </row>
+    <row r="35" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M35" s="11"/>
+    </row>
+    <row r="36" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M36" s="11"/>
+    </row>
+    <row r="37" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M37" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M60:N1048576">
-      <formula1>$E$4:$E$19</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O60:P1048576">
+      <formula1>$G$4:$G$19</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="P4" r:id="rId1"/>
-    <hyperlink ref="P2" r:id="rId2"/>
-    <hyperlink ref="P3" r:id="rId3"/>
+    <hyperlink ref="R4" r:id="rId1"/>
+    <hyperlink ref="R2" r:id="rId2"/>
+    <hyperlink ref="R3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1164,31 +1217,31 @@
           <x14:formula1>
             <xm:f>ValidationLists!$A$2:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
+          <xm:sqref>K2:K1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ValidationLists!$C$2:$C$10</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ValidationLists!$D$2:$D$14</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:K1048576</xm:sqref>
+          <xm:sqref>L2:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ValidationLists!$E$2:$E$19</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
+          <xm:sqref>N2:N1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ValidationLists!$F$2:$F$16</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:N59</xm:sqref>
+          <xm:sqref>O2:P59</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1202,13 +1255,13 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K68" sqref="K68"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.5" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" style="13" customWidth="1"/>
     <col min="5" max="6" width="20" style="13" customWidth="1"/>
@@ -1220,44 +1273,44 @@
   <sheetData>
     <row r="1" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C1" s="12" t="str">
-        <f>'Plots - metadata'!I1</f>
+        <f>'Plots - metadata'!K1</f>
         <v>Condition</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>46</v>
+      <c r="L1" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -1266,22 +1319,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C2" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D2" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H2" s="13">
         <v>0</v>
@@ -1318,22 +1371,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C3" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D3" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H3" s="13">
         <v>1</v>
@@ -1366,22 +1419,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C4" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D4" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H4" s="13">
         <v>2</v>
@@ -1414,22 +1467,22 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C5" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D5" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H5" s="13">
         <v>3</v>
@@ -1462,22 +1515,22 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C6" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D6" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H6" s="13">
         <v>4</v>
@@ -1510,22 +1563,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C7" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D7" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H7" s="13">
         <v>5</v>
@@ -1558,22 +1611,22 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C8" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D8" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H8" s="13">
         <v>6</v>
@@ -1606,22 +1659,22 @@
         <v>1</v>
       </c>
       <c r="B9" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C9" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D9" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H9" s="13">
         <v>7</v>
@@ -1654,22 +1707,22 @@
         <v>1</v>
       </c>
       <c r="B10" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C10" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D10" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H10" s="13">
         <v>8</v>
@@ -1702,22 +1755,22 @@
         <v>1</v>
       </c>
       <c r="B11" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C11" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D11" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H11" s="13">
         <v>9</v>
@@ -1750,22 +1803,22 @@
         <v>1</v>
       </c>
       <c r="B12" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C12" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D12" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H12" s="13">
         <v>10</v>
@@ -1798,22 +1851,22 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C13" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D13" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H13" s="13">
         <v>0</v>
@@ -1851,22 +1904,22 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C14" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D14" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H14" s="13">
         <v>1</v>
@@ -1899,22 +1952,22 @@
         <v>1</v>
       </c>
       <c r="B15" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C15" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D15" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H15" s="13">
         <v>2</v>
@@ -1947,22 +2000,22 @@
         <v>1</v>
       </c>
       <c r="B16" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C16" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D16" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H16" s="13">
         <v>3</v>
@@ -1995,22 +2048,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C17" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D17" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H17" s="13">
         <v>4</v>
@@ -2043,22 +2096,22 @@
         <v>1</v>
       </c>
       <c r="B18" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C18" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D18" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H18" s="13">
         <v>5</v>
@@ -2091,22 +2144,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C19" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D19" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H19" s="13">
         <v>6</v>
@@ -2139,22 +2192,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C20" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D20" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H20" s="13">
         <v>7</v>
@@ -2187,22 +2240,22 @@
         <v>1</v>
       </c>
       <c r="B21" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C21" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D21" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H21" s="13">
         <v>8</v>
@@ -2235,22 +2288,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C22" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D22" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H22" s="13">
         <v>9</v>
@@ -2283,22 +2336,22 @@
         <v>1</v>
       </c>
       <c r="B23" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C23" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D23" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H23" s="13">
         <v>10</v>
@@ -2331,22 +2384,22 @@
         <v>1</v>
       </c>
       <c r="B24" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C24" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D24" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H24" s="13">
         <v>0</v>
@@ -2379,22 +2432,22 @@
         <v>1</v>
       </c>
       <c r="B25" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C25" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D25" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H25" s="13">
         <v>1</v>
@@ -2427,22 +2480,22 @@
         <v>1</v>
       </c>
       <c r="B26" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C26" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D26" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H26" s="13">
         <v>2</v>
@@ -2475,22 +2528,22 @@
         <v>1</v>
       </c>
       <c r="B27" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C27" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D27" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H27" s="13">
         <v>3</v>
@@ -2523,22 +2576,22 @@
         <v>1</v>
       </c>
       <c r="B28" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C28" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D28" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H28" s="13">
         <v>4</v>
@@ -2571,22 +2624,22 @@
         <v>1</v>
       </c>
       <c r="B29" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C29" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D29" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H29" s="13">
         <v>5</v>
@@ -2619,22 +2672,22 @@
         <v>1</v>
       </c>
       <c r="B30" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C30" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D30" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H30" s="13">
         <v>6</v>
@@ -2667,22 +2720,22 @@
         <v>1</v>
       </c>
       <c r="B31" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C31" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D31" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H31" s="13">
         <v>7</v>
@@ -2715,22 +2768,22 @@
         <v>1</v>
       </c>
       <c r="B32" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C32" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D32" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H32" s="13">
         <v>8</v>
@@ -2763,22 +2816,22 @@
         <v>1</v>
       </c>
       <c r="B33" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C33" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D33" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H33" s="13">
         <v>9</v>
@@ -2811,22 +2864,22 @@
         <v>1</v>
       </c>
       <c r="B34" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C34" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D34" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H34" s="13">
         <v>10</v>
@@ -2859,22 +2912,22 @@
         <v>1</v>
       </c>
       <c r="B35" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C35" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D35" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H35" s="13">
         <v>0</v>
@@ -2907,22 +2960,22 @@
         <v>1</v>
       </c>
       <c r="B36" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C36" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D36" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H36" s="13">
         <v>1</v>
@@ -2953,22 +3006,22 @@
         <v>1</v>
       </c>
       <c r="B37" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C37" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D37" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H37" s="13">
         <v>2</v>
@@ -2999,22 +3052,22 @@
         <v>1</v>
       </c>
       <c r="B38" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C38" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D38" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H38" s="13">
         <v>3</v>
@@ -3045,22 +3098,22 @@
         <v>1</v>
       </c>
       <c r="B39" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C39" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D39" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H39" s="13">
         <v>4</v>
@@ -3091,22 +3144,22 @@
         <v>1</v>
       </c>
       <c r="B40" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C40" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D40" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H40" s="13">
         <v>5</v>
@@ -3137,22 +3190,22 @@
         <v>1</v>
       </c>
       <c r="B41" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C41" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D41" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H41" s="13">
         <v>6</v>
@@ -3183,22 +3236,22 @@
         <v>1</v>
       </c>
       <c r="B42" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C42" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D42" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H42" s="13">
         <v>7</v>
@@ -3229,22 +3282,22 @@
         <v>1</v>
       </c>
       <c r="B43" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C43" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D43" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H43" s="13">
         <v>8</v>
@@ -3275,22 +3328,22 @@
         <v>1</v>
       </c>
       <c r="B44" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C44" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D44" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H44" s="13">
         <v>9</v>
@@ -3321,22 +3374,22 @@
         <v>1</v>
       </c>
       <c r="B45" s="7" t="str">
-        <f>'Plots - metadata'!$C$2</f>
-        <v>Ovarian cancer 10-yr overall survival</v>
+        <f>'Plots - metadata'!$E$2</f>
+        <v>Ovarian cancer 10-yr overall survival (SEER 1988-2001)</v>
       </c>
       <c r="C45" s="13" t="str">
-        <f>'Plots - metadata'!$I$2</f>
+        <f>'Plots - metadata'!$K$2</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D45" s="13" t="str">
-        <f>'Plots - metadata'!$L$2</f>
+        <f>'Plots - metadata'!$N$2</f>
         <v>Overall survival</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H45" s="13">
         <v>10</v>
@@ -3367,22 +3420,22 @@
         <v>1</v>
       </c>
       <c r="B47" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C47" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D47" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H47" s="13">
         <v>0</v>
@@ -3413,22 +3466,22 @@
         <v>1</v>
       </c>
       <c r="B48" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C48" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D48" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H48" s="13">
         <v>1</v>
@@ -3459,22 +3512,22 @@
         <v>1</v>
       </c>
       <c r="B49" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C49" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D49" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H49" s="13">
         <v>2</v>
@@ -3505,22 +3558,22 @@
         <v>1</v>
       </c>
       <c r="B50" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C50" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D50" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H50" s="13">
         <v>3</v>
@@ -3551,22 +3604,22 @@
         <v>1</v>
       </c>
       <c r="B51" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C51" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D51" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H51" s="13">
         <v>4</v>
@@ -3597,22 +3650,22 @@
         <v>1</v>
       </c>
       <c r="B52" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C52" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D52" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H52" s="13">
         <v>5</v>
@@ -3643,22 +3696,22 @@
         <v>1</v>
       </c>
       <c r="B53" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C53" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D53" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H53" s="13">
         <v>0</v>
@@ -3689,22 +3742,22 @@
         <v>1</v>
       </c>
       <c r="B54" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C54" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D54" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H54" s="13">
         <v>1</v>
@@ -3735,22 +3788,22 @@
         <v>1</v>
       </c>
       <c r="B55" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C55" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D55" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H55" s="13">
         <v>2</v>
@@ -3781,22 +3834,22 @@
         <v>1</v>
       </c>
       <c r="B56" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C56" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D56" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H56" s="13">
         <v>3</v>
@@ -3827,22 +3880,22 @@
         <v>1</v>
       </c>
       <c r="B57" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C57" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D57" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H57" s="13">
         <v>4</v>
@@ -3873,22 +3926,22 @@
         <v>1</v>
       </c>
       <c r="B58" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C58" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D58" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H58" s="13">
         <v>5</v>
@@ -3919,22 +3972,22 @@
         <v>1</v>
       </c>
       <c r="B59" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C59" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D59" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H59" s="13">
         <v>0</v>
@@ -3965,22 +4018,22 @@
         <v>1</v>
       </c>
       <c r="B60" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C60" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D60" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E60" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H60" s="13">
         <v>1</v>
@@ -4011,22 +4064,22 @@
         <v>1</v>
       </c>
       <c r="B61" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C61" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D61" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H61" s="13">
         <v>2</v>
@@ -4057,22 +4110,22 @@
         <v>1</v>
       </c>
       <c r="B62" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C62" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D62" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H62" s="13">
         <v>3</v>
@@ -4103,22 +4156,22 @@
         <v>1</v>
       </c>
       <c r="B63" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C63" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D63" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H63" s="13">
         <v>4</v>
@@ -4149,22 +4202,22 @@
         <v>1</v>
       </c>
       <c r="B64" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C64" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D64" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H64" s="13">
         <v>5</v>
@@ -4195,22 +4248,22 @@
         <v>1</v>
       </c>
       <c r="B65" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C65" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D65" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H65" s="13">
         <v>0</v>
@@ -4241,22 +4294,22 @@
         <v>1</v>
       </c>
       <c r="B66" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C66" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D66" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H66" s="13">
         <v>1</v>
@@ -4287,22 +4340,22 @@
         <v>1</v>
       </c>
       <c r="B67" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C67" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D67" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H67" s="13">
         <v>2</v>
@@ -4333,22 +4386,22 @@
         <v>1</v>
       </c>
       <c r="B68" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C68" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D68" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H68" s="13">
         <v>3</v>
@@ -4379,22 +4432,22 @@
         <v>1</v>
       </c>
       <c r="B69" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C69" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D69" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F69" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H69" s="13">
         <v>4</v>
@@ -4425,22 +4478,22 @@
         <v>1</v>
       </c>
       <c r="B70" s="7" t="str">
-        <f>'Plots - metadata'!$C$3</f>
-        <v>Ovarian cancer 5-yr conditional survival by stage</v>
+        <f>'Plots - metadata'!$E$3</f>
+        <v>Ovarian cancer 5-yr conditional survival by stage (SEER 1988-2001)</v>
       </c>
       <c r="C70" s="13" t="str">
-        <f>'Plots - metadata'!$I$3</f>
+        <f>'Plots - metadata'!$K$3</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D70" s="13" t="str">
-        <f>'Plots - metadata'!$D$3</f>
+        <f>'Plots - metadata'!$F$3</f>
         <v>Conditional survival</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H70" s="13">
         <v>5</v>
@@ -4475,25 +4528,25 @@
         <v>1</v>
       </c>
       <c r="B72" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C72" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D72" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G72" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H72" s="13">
         <v>0</v>
@@ -4520,25 +4573,25 @@
         <v>1</v>
       </c>
       <c r="B73" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C73" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D73" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G73" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H73" s="13">
         <v>1</v>
@@ -4565,25 +4618,25 @@
         <v>1</v>
       </c>
       <c r="B74" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C74" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D74" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H74" s="13">
         <v>2</v>
@@ -4610,25 +4663,25 @@
         <v>1</v>
       </c>
       <c r="B75" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C75" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D75" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H75" s="13">
         <v>3</v>
@@ -4655,25 +4708,25 @@
         <v>1</v>
       </c>
       <c r="B76" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C76" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D76" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H76" s="13">
         <v>4</v>
@@ -4700,25 +4753,25 @@
         <v>1</v>
       </c>
       <c r="B77" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C77" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D77" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H77" s="13">
         <v>5</v>
@@ -4745,25 +4798,25 @@
         <v>1</v>
       </c>
       <c r="B78" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C78" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D78" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G78" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H78" s="13">
         <v>0</v>
@@ -4790,25 +4843,25 @@
         <v>1</v>
       </c>
       <c r="B79" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C79" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D79" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G79" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H79" s="13">
         <v>1</v>
@@ -4835,25 +4888,25 @@
         <v>1</v>
       </c>
       <c r="B80" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C80" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D80" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G80" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H80" s="13">
         <v>2</v>
@@ -4880,25 +4933,25 @@
         <v>1</v>
       </c>
       <c r="B81" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C81" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D81" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G81" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H81" s="13">
         <v>3</v>
@@ -4925,25 +4978,25 @@
         <v>1</v>
       </c>
       <c r="B82" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C82" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D82" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G82" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H82" s="13">
         <v>4</v>
@@ -4970,25 +5023,25 @@
         <v>1</v>
       </c>
       <c r="B83" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C83" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D83" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G83" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H83" s="13">
         <v>5</v>
@@ -5015,25 +5068,25 @@
         <v>1</v>
       </c>
       <c r="B84" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C84" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D84" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E84" s="13" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G84" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H84" s="13">
         <v>0</v>
@@ -5060,25 +5113,25 @@
         <v>1</v>
       </c>
       <c r="B85" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C85" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D85" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G85" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H85" s="13">
         <v>1</v>
@@ -5105,25 +5158,25 @@
         <v>1</v>
       </c>
       <c r="B86" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C86" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D86" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G86" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H86" s="13">
         <v>2</v>
@@ -5150,25 +5203,25 @@
         <v>1</v>
       </c>
       <c r="B87" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C87" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D87" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G87" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H87" s="13">
         <v>3</v>
@@ -5195,25 +5248,25 @@
         <v>1</v>
       </c>
       <c r="B88" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C88" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D88" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G88" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H88" s="13">
         <v>4</v>
@@ -5240,25 +5293,25 @@
         <v>1</v>
       </c>
       <c r="B89" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C89" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D89" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E89" s="13" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G89" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H89" s="13">
         <v>5</v>
@@ -5285,25 +5338,25 @@
         <v>1</v>
       </c>
       <c r="B90" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C90" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D90" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G90" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H90" s="13">
         <v>0</v>
@@ -5330,25 +5383,25 @@
         <v>1</v>
       </c>
       <c r="B91" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C91" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D91" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G91" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H91" s="13">
         <v>1</v>
@@ -5375,25 +5428,25 @@
         <v>1</v>
       </c>
       <c r="B92" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C92" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D92" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G92" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H92" s="13">
         <v>2</v>
@@ -5420,25 +5473,25 @@
         <v>1</v>
       </c>
       <c r="B93" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C93" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D93" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G93" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H93" s="13">
         <v>3</v>
@@ -5465,25 +5518,25 @@
         <v>1</v>
       </c>
       <c r="B94" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C94" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D94" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G94" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H94" s="13">
         <v>4</v>
@@ -5510,25 +5563,25 @@
         <v>1</v>
       </c>
       <c r="B95" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C95" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D95" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G95" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H95" s="13">
         <v>5</v>
@@ -5555,25 +5608,25 @@
         <v>1</v>
       </c>
       <c r="B96" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C96" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D96" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G96" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H96" s="13">
         <v>0</v>
@@ -5600,25 +5653,25 @@
         <v>1</v>
       </c>
       <c r="B97" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C97" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D97" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G97" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H97" s="13">
         <v>1</v>
@@ -5645,25 +5698,25 @@
         <v>1</v>
       </c>
       <c r="B98" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C98" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D98" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G98" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H98" s="13">
         <v>2</v>
@@ -5690,25 +5743,25 @@
         <v>1</v>
       </c>
       <c r="B99" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C99" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D99" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G99" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H99" s="13">
         <v>3</v>
@@ -5735,25 +5788,25 @@
         <v>1</v>
       </c>
       <c r="B100" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C100" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D100" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H100" s="13">
         <v>4</v>
@@ -5780,25 +5833,25 @@
         <v>1</v>
       </c>
       <c r="B101" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C101" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D101" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G101" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H101" s="13">
         <v>5</v>
@@ -5825,25 +5878,25 @@
         <v>1</v>
       </c>
       <c r="B102" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C102" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D102" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F102" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G102" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H102" s="13">
         <v>0</v>
@@ -5870,25 +5923,25 @@
         <v>1</v>
       </c>
       <c r="B103" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C103" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D103" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F103" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G103" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H103" s="13">
         <v>1</v>
@@ -5915,25 +5968,25 @@
         <v>1</v>
       </c>
       <c r="B104" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C104" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D104" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F104" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G104" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H104" s="13">
         <v>2</v>
@@ -5960,25 +6013,25 @@
         <v>1</v>
       </c>
       <c r="B105" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C105" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D105" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F105" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G105" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H105" s="13">
         <v>3</v>
@@ -6005,25 +6058,25 @@
         <v>1</v>
       </c>
       <c r="B106" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C106" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D106" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E106" s="13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F106" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H106" s="13">
         <v>4</v>
@@ -6050,25 +6103,25 @@
         <v>1</v>
       </c>
       <c r="B107" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C107" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D107" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E107" s="13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F107" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H107" s="13">
         <v>5</v>
@@ -6095,25 +6148,25 @@
         <v>1</v>
       </c>
       <c r="B108" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C108" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D108" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E108" s="13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F108" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G108" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H108" s="13">
         <v>0</v>
@@ -6140,25 +6193,25 @@
         <v>1</v>
       </c>
       <c r="B109" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C109" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D109" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E109" s="13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F109" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G109" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H109" s="13">
         <v>1</v>
@@ -6185,25 +6238,25 @@
         <v>1</v>
       </c>
       <c r="B110" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C110" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D110" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E110" s="13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F110" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G110" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H110" s="13">
         <v>2</v>
@@ -6230,25 +6283,25 @@
         <v>1</v>
       </c>
       <c r="B111" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C111" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D111" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E111" s="13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F111" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G111" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H111" s="13">
         <v>3</v>
@@ -6275,25 +6328,25 @@
         <v>1</v>
       </c>
       <c r="B112" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C112" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D112" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E112" s="13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F112" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G112" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H112" s="13">
         <v>4</v>
@@ -6320,25 +6373,25 @@
         <v>1</v>
       </c>
       <c r="B113" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C113" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D113" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E113" s="13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F113" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G113" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H113" s="13">
         <v>5</v>
@@ -6365,25 +6418,25 @@
         <v>1</v>
       </c>
       <c r="B114" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C114" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D114" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F114" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G114" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H114" s="13">
         <v>0</v>
@@ -6410,25 +6463,25 @@
         <v>1</v>
       </c>
       <c r="B115" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C115" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D115" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F115" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G115" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H115" s="13">
         <v>1</v>
@@ -6455,25 +6508,25 @@
         <v>1</v>
       </c>
       <c r="B116" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C116" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D116" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F116" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G116" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H116" s="13">
         <v>2</v>
@@ -6500,25 +6553,25 @@
         <v>1</v>
       </c>
       <c r="B117" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C117" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D117" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F117" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G117" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H117" s="13">
         <v>3</v>
@@ -6545,25 +6598,25 @@
         <v>1</v>
       </c>
       <c r="B118" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C118" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D118" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E118" s="13" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F118" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G118" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H118" s="13">
         <v>4</v>
@@ -6590,25 +6643,25 @@
         <v>1</v>
       </c>
       <c r="B119" s="7" t="str">
-        <f>'Plots - metadata'!$C$4</f>
-        <v>Ovarian cancer 5-yr conditional survival by age-group and stage</v>
+        <f>'Plots - metadata'!$E$4</f>
+        <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="C119" s="13" t="str">
-        <f>'Plots - metadata'!$I$4</f>
+        <f>'Plots - metadata'!$K$4</f>
         <v>Ovarian cancer</v>
       </c>
       <c r="D119" s="13" t="str">
-        <f>'Plots - metadata'!$L$4</f>
+        <f>'Plots - metadata'!$N$4</f>
         <v>Overall survival</v>
       </c>
       <c r="E119" s="13" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F119" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G119" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H119" s="13">
         <v>5</v>
@@ -7378,19 +7431,19 @@
         <v>9</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -7398,21 +7451,21 @@
         <v>0</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>20</v>
@@ -7421,7 +7474,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweak to legend title
</commit_message>
<xml_diff>
--- a/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
+++ b/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
@@ -358,7 +358,8 @@
     <t>title4Legend</t>
   </si>
   <si>
-    <t>Stage and\nage group</t>
+    <t>Stage and
+age group</t>
   </si>
 </sst>
 </file>
@@ -789,7 +790,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adjusted widths of CI and BW ranges
</commit_message>
<xml_diff>
--- a/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
+++ b/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="plotsMetadata" sheetId="9" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="110">
   <si>
     <t>Ovarian cancer</t>
   </si>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t>Outcomes</t>
-  </si>
-  <si>
-    <t>Ten-year (relative) overall survival curves in ovarian cancer patients by stage.</t>
   </si>
   <si>
     <t>Ovarian cancer 10-yr overall survival</t>
@@ -360,6 +357,15 @@
   <si>
     <t>Stage and
 age group</t>
+  </si>
+  <si>
+    <t>Ten-year (relative) overall survival curves in ovarian cancer by stage.</t>
+  </si>
+  <si>
+    <t>wbWidth</t>
+  </si>
+  <si>
+    <t>ciWidth</t>
   </si>
 </sst>
 </file>
@@ -426,12 +432,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -507,9 +514,28 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -788,9 +814,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -800,7 +826,7 @@
     <col min="3" max="3" width="6.1640625" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="32.33203125" style="16" customWidth="1"/>
     <col min="7" max="7" width="17" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.6640625" style="30" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.5" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="44.83203125" style="7" customWidth="1"/>
@@ -818,64 +844,64 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="H1" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="I1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="U1" s="6"/>
     </row>
@@ -887,10 +913,10 @@
         <v>47</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="17" t="str">
         <f>CONCATENATE(D2," (",B2,")")</f>
@@ -902,17 +928,17 @@
       <c r="G2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>64</v>
+      <c r="H2" s="27" t="s">
+        <v>107</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>49</v>
       </c>
       <c r="J2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>0</v>
@@ -949,10 +975,10 @@
         <v>47</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="17" t="str">
         <f t="shared" ref="E3:E4" si="0">CONCATENATE(D3," (",B3,")")</f>
@@ -964,8 +990,8 @@
       <c r="G3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>74</v>
+      <c r="H3" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>49</v>
@@ -1011,22 +1037,22 @@
         <v>47</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="27" t="s">
         <v>48</v>
       </c>
       <c r="I4" s="8" t="s">
@@ -1068,6 +1094,7 @@
       <c r="U4" s="19"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="H5" s="28"/>
       <c r="M5" s="11"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -1122,7 +1149,7 @@
       <c r="Q14" s="11"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="H16" s="11"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
@@ -1135,7 +1162,7 @@
       <c r="U16" s="10"/>
     </row>
     <row r="17" spans="8:21" x14ac:dyDescent="0.2">
-      <c r="H17" s="11"/>
+      <c r="H17" s="31"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
@@ -1148,7 +1175,7 @@
       <c r="U17" s="10"/>
     </row>
     <row r="20" spans="8:21" x14ac:dyDescent="0.2">
-      <c r="H20" s="11"/>
+      <c r="H20" s="31"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
@@ -1161,7 +1188,7 @@
       <c r="U20" s="10"/>
     </row>
     <row r="21" spans="8:21" x14ac:dyDescent="0.2">
-      <c r="H21" s="11"/>
+      <c r="H21" s="31"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
@@ -1174,7 +1201,7 @@
       <c r="U21" s="10"/>
     </row>
     <row r="24" spans="8:21" x14ac:dyDescent="0.2">
-      <c r="H24" s="11"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
@@ -1187,7 +1214,7 @@
       <c r="U24" s="10"/>
     </row>
     <row r="25" spans="8:21" x14ac:dyDescent="0.2">
-      <c r="H25" s="11"/>
+      <c r="H25" s="31"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
@@ -1275,9 +1302,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomLeft" activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1311,31 +1338,31 @@
         <v>outcome</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>97</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>98</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>38</v>
       </c>
       <c r="I1" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="M1" s="26" t="s">
         <v>102</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -1368,23 +1395,27 @@
         <v>1</v>
       </c>
       <c r="J2" s="22">
-        <f>MIN(1, I2*0.85)</f>
-        <v>0.85</v>
+        <f>MAX(0,I2*(1-$P$2))</f>
+        <v>0.9</v>
       </c>
       <c r="K2" s="22">
-        <f>MIN(1, I2*1.15)</f>
+        <f>MIN(1,I2*(1+$P$2))</f>
         <v>1</v>
       </c>
       <c r="L2" s="22">
-        <f>MIN(1, J2*0.85)</f>
-        <v>0.72249999999999992</v>
+        <f>MAX(0,I2*(1-$P$3))</f>
+        <v>0.8</v>
       </c>
       <c r="M2" s="22">
-        <f>MIN(1, K2*1.15)</f>
-        <v>1</v>
-      </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="4"/>
+        <f>MIN(1,I2*(1+$P$3))</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="P2" s="32">
+        <v>0.1</v>
+      </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
@@ -1420,20 +1451,26 @@
         <v>0.96</v>
       </c>
       <c r="J3" s="22">
-        <f t="shared" ref="J3:J66" si="0">MIN(1, I3*0.85)</f>
-        <v>0.81599999999999995</v>
+        <f t="shared" ref="J3:J66" si="0">MAX(0,I3*(1-$P$2))</f>
+        <v>0.86399999999999999</v>
       </c>
       <c r="K3" s="22">
-        <f t="shared" ref="K3:K45" si="1">MIN(1, I3*1.15)</f>
+        <f t="shared" ref="K3:K45" si="1">MIN(1,I3*(1+$P$2))</f>
         <v>1</v>
       </c>
       <c r="L3" s="22">
-        <f t="shared" ref="L3:L45" si="2">MIN(1, J3*0.85)</f>
-        <v>0.69359999999999988</v>
+        <f t="shared" ref="L3:L45" si="2">MAX(0,I3*(1-$P$3))</f>
+        <v>0.76800000000000002</v>
       </c>
       <c r="M3" s="22">
-        <f t="shared" ref="M3:M45" si="3">MIN(1, K3*1.15)</f>
-        <v>1</v>
+        <f t="shared" ref="M3:M45" si="3">MIN(1,I3*(1+$P$3))</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="P3" s="32">
+        <v>0.2</v>
       </c>
       <c r="S3" s="14"/>
       <c r="T3" s="14"/>
@@ -1469,7 +1506,7 @@
       </c>
       <c r="J4" s="22">
         <f t="shared" si="0"/>
-        <v>0.79899999999999993</v>
+        <v>0.84599999999999997</v>
       </c>
       <c r="K4" s="22">
         <f t="shared" si="1"/>
@@ -1477,7 +1514,7 @@
       </c>
       <c r="L4" s="22">
         <f t="shared" si="2"/>
-        <v>0.67914999999999992</v>
+        <v>0.752</v>
       </c>
       <c r="M4" s="22">
         <f t="shared" si="3"/>
@@ -1517,7 +1554,7 @@
       </c>
       <c r="J5" s="22">
         <f t="shared" si="0"/>
-        <v>0.78200000000000003</v>
+        <v>0.82800000000000007</v>
       </c>
       <c r="K5" s="22">
         <f t="shared" si="1"/>
@@ -1525,7 +1562,7 @@
       </c>
       <c r="L5" s="22">
         <f t="shared" si="2"/>
-        <v>0.66469999999999996</v>
+        <v>0.7360000000000001</v>
       </c>
       <c r="M5" s="22">
         <f t="shared" si="3"/>
@@ -1565,15 +1602,15 @@
       </c>
       <c r="J6" s="22">
         <f t="shared" si="0"/>
-        <v>0.76500000000000001</v>
+        <v>0.81</v>
       </c>
       <c r="K6" s="22">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.9900000000000001</v>
       </c>
       <c r="L6" s="22">
         <f t="shared" si="2"/>
-        <v>0.65024999999999999</v>
+        <v>0.72000000000000008</v>
       </c>
       <c r="M6" s="22">
         <f t="shared" si="3"/>
@@ -1613,15 +1650,15 @@
       </c>
       <c r="J7" s="22">
         <f t="shared" si="0"/>
-        <v>0.75649999999999995</v>
+        <v>0.80100000000000005</v>
       </c>
       <c r="K7" s="22">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.97900000000000009</v>
       </c>
       <c r="L7" s="22">
         <f t="shared" si="2"/>
-        <v>0.64302499999999996</v>
+        <v>0.71200000000000008</v>
       </c>
       <c r="M7" s="22">
         <f t="shared" si="3"/>
@@ -1661,15 +1698,15 @@
       </c>
       <c r="J8" s="22">
         <f t="shared" si="0"/>
-        <v>0.748</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="K8" s="22">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.96800000000000008</v>
       </c>
       <c r="L8" s="22">
         <f t="shared" si="2"/>
-        <v>0.63580000000000003</v>
+        <v>0.70400000000000007</v>
       </c>
       <c r="M8" s="22">
         <f t="shared" si="3"/>
@@ -1709,15 +1746,15 @@
       </c>
       <c r="J9" s="22">
         <f t="shared" si="0"/>
-        <v>0.73949999999999994</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="K9" s="22">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.95700000000000007</v>
       </c>
       <c r="L9" s="22">
         <f t="shared" si="2"/>
-        <v>0.62857499999999988</v>
+        <v>0.69600000000000006</v>
       </c>
       <c r="M9" s="22">
         <f t="shared" si="3"/>
@@ -1757,15 +1794,15 @@
       </c>
       <c r="J10" s="22">
         <f t="shared" si="0"/>
-        <v>0.73099999999999998</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="K10" s="22">
         <f t="shared" si="1"/>
-        <v>0.98899999999999988</v>
+        <v>0.94600000000000006</v>
       </c>
       <c r="L10" s="22">
         <f t="shared" si="2"/>
-        <v>0.62134999999999996</v>
+        <v>0.68800000000000006</v>
       </c>
       <c r="M10" s="22">
         <f t="shared" si="3"/>
@@ -1805,15 +1842,15 @@
       </c>
       <c r="J11" s="22">
         <f t="shared" si="0"/>
-        <v>0.72675000000000001</v>
+        <v>0.76949999999999996</v>
       </c>
       <c r="K11" s="22">
         <f t="shared" si="1"/>
-        <v>0.98324999999999996</v>
+        <v>0.9405</v>
       </c>
       <c r="L11" s="22">
         <f t="shared" si="2"/>
-        <v>0.61773749999999994</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="M11" s="22">
         <f t="shared" si="3"/>
@@ -1853,15 +1890,15 @@
       </c>
       <c r="J12" s="22">
         <f t="shared" si="0"/>
-        <v>0.72249999999999992</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="K12" s="22">
         <f t="shared" si="1"/>
-        <v>0.97749999999999992</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="L12" s="22">
         <f t="shared" si="2"/>
-        <v>0.61412499999999992</v>
+        <v>0.68</v>
       </c>
       <c r="M12" s="22">
         <f t="shared" si="3"/>
@@ -1901,7 +1938,7 @@
       </c>
       <c r="J13" s="22">
         <f t="shared" si="0"/>
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="K13" s="22">
         <f t="shared" si="1"/>
@@ -1909,7 +1946,7 @@
       </c>
       <c r="L13" s="22">
         <f t="shared" si="2"/>
-        <v>0.72249999999999992</v>
+        <v>0.8</v>
       </c>
       <c r="M13" s="22">
         <f t="shared" si="3"/>
@@ -1954,15 +1991,15 @@
       </c>
       <c r="J14" s="22">
         <f t="shared" si="0"/>
-        <v>0.73099999999999998</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="K14" s="22">
         <f t="shared" si="1"/>
-        <v>0.98899999999999988</v>
+        <v>0.94600000000000006</v>
       </c>
       <c r="L14" s="22">
         <f t="shared" si="2"/>
-        <v>0.62134999999999996</v>
+        <v>0.68800000000000006</v>
       </c>
       <c r="M14" s="22">
         <f t="shared" si="3"/>
@@ -2002,19 +2039,19 @@
       </c>
       <c r="J15" s="22">
         <f t="shared" si="0"/>
-        <v>0.64600000000000002</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="K15" s="22">
         <f t="shared" si="1"/>
-        <v>0.87399999999999989</v>
+        <v>0.83600000000000008</v>
       </c>
       <c r="L15" s="22">
         <f t="shared" si="2"/>
-        <v>0.54910000000000003</v>
+        <v>0.6080000000000001</v>
       </c>
       <c r="M15" s="22">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.91199999999999992</v>
       </c>
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
@@ -2050,19 +2087,19 @@
       </c>
       <c r="J16" s="22">
         <f t="shared" si="0"/>
-        <v>0.62049999999999994</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="K16" s="22">
         <f t="shared" si="1"/>
-        <v>0.83949999999999991</v>
+        <v>0.80300000000000005</v>
       </c>
       <c r="L16" s="22">
         <f t="shared" si="2"/>
-        <v>0.52742499999999992</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="M16" s="22">
         <f t="shared" si="3"/>
-        <v>0.96542499999999987</v>
+        <v>0.876</v>
       </c>
       <c r="S16" s="14"/>
       <c r="T16" s="14"/>
@@ -2098,19 +2135,19 @@
       </c>
       <c r="J17" s="22">
         <f t="shared" si="0"/>
-        <v>0.58649999999999991</v>
+        <v>0.621</v>
       </c>
       <c r="K17" s="22">
         <f t="shared" si="1"/>
-        <v>0.79349999999999987</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="L17" s="22">
         <f t="shared" si="2"/>
-        <v>0.49852499999999988</v>
+        <v>0.55199999999999994</v>
       </c>
       <c r="M17" s="22">
         <f t="shared" si="3"/>
-        <v>0.91252499999999981</v>
+        <v>0.82799999999999996</v>
       </c>
       <c r="S17" s="14"/>
       <c r="T17" s="14"/>
@@ -2146,19 +2183,19 @@
       </c>
       <c r="J18" s="22">
         <f t="shared" si="0"/>
-        <v>0.56950000000000001</v>
+        <v>0.60300000000000009</v>
       </c>
       <c r="K18" s="22">
         <f t="shared" si="1"/>
-        <v>0.77049999999999996</v>
+        <v>0.7370000000000001</v>
       </c>
       <c r="L18" s="22">
         <f t="shared" si="2"/>
-        <v>0.48407499999999998</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="M18" s="22">
         <f t="shared" si="3"/>
-        <v>0.88607499999999983</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="S18" s="14"/>
       <c r="T18" s="14"/>
@@ -2194,19 +2231,19 @@
       </c>
       <c r="J19" s="22">
         <f t="shared" si="0"/>
-        <v>0.55249999999999999</v>
+        <v>0.58500000000000008</v>
       </c>
       <c r="K19" s="22">
         <f t="shared" si="1"/>
-        <v>0.74749999999999994</v>
+        <v>0.71500000000000008</v>
       </c>
       <c r="L19" s="22">
         <f t="shared" si="2"/>
-        <v>0.46962499999999996</v>
+        <v>0.52</v>
       </c>
       <c r="M19" s="22">
         <f t="shared" si="3"/>
-        <v>0.85962499999999986</v>
+        <v>0.78</v>
       </c>
       <c r="S19" s="14"/>
       <c r="T19" s="14"/>
@@ -2242,19 +2279,19 @@
       </c>
       <c r="J20" s="22">
         <f t="shared" si="0"/>
-        <v>0.53549999999999998</v>
+        <v>0.56700000000000006</v>
       </c>
       <c r="K20" s="22">
         <f t="shared" si="1"/>
-        <v>0.72449999999999992</v>
+        <v>0.69300000000000006</v>
       </c>
       <c r="L20" s="22">
         <f t="shared" si="2"/>
-        <v>0.45517499999999994</v>
+        <v>0.504</v>
       </c>
       <c r="M20" s="22">
         <f t="shared" si="3"/>
-        <v>0.83317499999999989</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="S20" s="14"/>
       <c r="T20" s="14"/>
@@ -2290,19 +2327,19 @@
       </c>
       <c r="J21" s="22">
         <f t="shared" si="0"/>
-        <v>0.52700000000000002</v>
+        <v>0.55800000000000005</v>
       </c>
       <c r="K21" s="22">
         <f t="shared" si="1"/>
-        <v>0.71299999999999997</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="L21" s="22">
         <f t="shared" si="2"/>
-        <v>0.44795000000000001</v>
+        <v>0.496</v>
       </c>
       <c r="M21" s="22">
         <f t="shared" si="3"/>
-        <v>0.81994999999999985</v>
+        <v>0.74399999999999999</v>
       </c>
       <c r="S21" s="14"/>
       <c r="T21" s="14"/>
@@ -2338,19 +2375,19 @@
       </c>
       <c r="J22" s="22">
         <f t="shared" si="0"/>
-        <v>0.51849999999999996</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="K22" s="22">
         <f t="shared" si="1"/>
-        <v>0.7014999999999999</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="L22" s="22">
         <f t="shared" si="2"/>
-        <v>0.44072499999999998</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="M22" s="22">
         <f t="shared" si="3"/>
-        <v>0.8067249999999998</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="S22" s="14"/>
       <c r="T22" s="14"/>
@@ -2386,19 +2423,19 @@
       </c>
       <c r="J23" s="22">
         <f t="shared" si="0"/>
-        <v>0.51424999999999998</v>
+        <v>0.54449999999999998</v>
       </c>
       <c r="K23" s="22">
         <f t="shared" si="1"/>
-        <v>0.69574999999999998</v>
+        <v>0.66549999999999998</v>
       </c>
       <c r="L23" s="22">
         <f t="shared" si="2"/>
-        <v>0.43711249999999996</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="M23" s="22">
         <f t="shared" si="3"/>
-        <v>0.80011249999999989</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="S23" s="14"/>
       <c r="T23" s="14"/>
@@ -2434,7 +2471,7 @@
       </c>
       <c r="J24" s="22">
         <f t="shared" si="0"/>
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="K24" s="22">
         <f t="shared" si="1"/>
@@ -2442,7 +2479,7 @@
       </c>
       <c r="L24" s="22">
         <f t="shared" si="2"/>
-        <v>0.72249999999999992</v>
+        <v>0.8</v>
       </c>
       <c r="M24" s="22">
         <f t="shared" si="3"/>
@@ -2482,19 +2519,19 @@
       </c>
       <c r="J25" s="22">
         <f t="shared" si="0"/>
-        <v>0.65449999999999997</v>
+        <v>0.69300000000000006</v>
       </c>
       <c r="K25" s="22">
         <f t="shared" si="1"/>
-        <v>0.88549999999999995</v>
+        <v>0.84700000000000009</v>
       </c>
       <c r="L25" s="22">
         <f t="shared" si="2"/>
-        <v>0.55632499999999996</v>
+        <v>0.6160000000000001</v>
       </c>
       <c r="M25" s="22">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.92399999999999993</v>
       </c>
       <c r="S25" s="14"/>
       <c r="T25" s="14"/>
@@ -2530,19 +2567,19 @@
       </c>
       <c r="J26" s="22">
         <f t="shared" si="0"/>
-        <v>0.53549999999999998</v>
+        <v>0.56700000000000006</v>
       </c>
       <c r="K26" s="22">
         <f t="shared" si="1"/>
-        <v>0.72449999999999992</v>
+        <v>0.69300000000000006</v>
       </c>
       <c r="L26" s="22">
         <f t="shared" si="2"/>
-        <v>0.45517499999999994</v>
+        <v>0.504</v>
       </c>
       <c r="M26" s="22">
         <f t="shared" si="3"/>
-        <v>0.83317499999999989</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="S26" s="14"/>
       <c r="T26" s="14"/>
@@ -2578,19 +2615,19 @@
       </c>
       <c r="J27" s="22">
         <f t="shared" si="0"/>
-        <v>0.4335</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="K27" s="22">
         <f t="shared" si="1"/>
-        <v>0.58649999999999991</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="L27" s="22">
         <f t="shared" si="2"/>
-        <v>0.368475</v>
+        <v>0.40800000000000003</v>
       </c>
       <c r="M27" s="22">
         <f t="shared" si="3"/>
-        <v>0.67447499999999982</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="S27" s="14"/>
       <c r="T27" s="14"/>
@@ -2626,19 +2663,19 @@
       </c>
       <c r="J28" s="22">
         <f t="shared" si="0"/>
-        <v>0.35699999999999998</v>
+        <v>0.378</v>
       </c>
       <c r="K28" s="22">
         <f t="shared" si="1"/>
-        <v>0.48299999999999993</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="L28" s="22">
         <f t="shared" si="2"/>
-        <v>0.30345</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="M28" s="22">
         <f t="shared" si="3"/>
-        <v>0.55544999999999989</v>
+        <v>0.504</v>
       </c>
       <c r="S28" s="14"/>
       <c r="T28" s="14"/>
@@ -2674,19 +2711,19 @@
       </c>
       <c r="J29" s="22">
         <f t="shared" si="0"/>
-        <v>0.28050000000000003</v>
+        <v>0.29700000000000004</v>
       </c>
       <c r="K29" s="22">
         <f t="shared" si="1"/>
-        <v>0.3795</v>
+        <v>0.36300000000000004</v>
       </c>
       <c r="L29" s="22">
         <f t="shared" si="2"/>
-        <v>0.23842500000000003</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="M29" s="22">
         <f t="shared" si="3"/>
-        <v>0.43642499999999995</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="S29" s="14"/>
       <c r="T29" s="14"/>
@@ -2722,19 +2759,19 @@
       </c>
       <c r="J30" s="22">
         <f t="shared" si="0"/>
-        <v>0.255</v>
+        <v>0.27</v>
       </c>
       <c r="K30" s="22">
         <f t="shared" si="1"/>
-        <v>0.34499999999999997</v>
+        <v>0.33</v>
       </c>
       <c r="L30" s="22">
         <f t="shared" si="2"/>
-        <v>0.21675</v>
+        <v>0.24</v>
       </c>
       <c r="M30" s="22">
         <f t="shared" si="3"/>
-        <v>0.39674999999999994</v>
+        <v>0.36</v>
       </c>
       <c r="S30" s="14"/>
       <c r="T30" s="14"/>
@@ -2770,19 +2807,19 @@
       </c>
       <c r="J31" s="22">
         <f t="shared" si="0"/>
-        <v>0.24649999999999997</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="K31" s="22">
         <f t="shared" si="1"/>
-        <v>0.33349999999999996</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="L31" s="22">
         <f t="shared" si="2"/>
-        <v>0.20952499999999996</v>
+        <v>0.23199999999999998</v>
       </c>
       <c r="M31" s="22">
         <f t="shared" si="3"/>
-        <v>0.38352499999999995</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="S31" s="14"/>
       <c r="T31" s="14"/>
@@ -2818,19 +2855,19 @@
       </c>
       <c r="J32" s="22">
         <f t="shared" si="0"/>
-        <v>0.22950000000000001</v>
+        <v>0.24300000000000002</v>
       </c>
       <c r="K32" s="22">
         <f t="shared" si="1"/>
-        <v>0.3105</v>
+        <v>0.29700000000000004</v>
       </c>
       <c r="L32" s="22">
         <f t="shared" si="2"/>
-        <v>0.195075</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="M32" s="22">
         <f t="shared" si="3"/>
-        <v>0.35707499999999998</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="S32" s="14"/>
       <c r="T32" s="14"/>
@@ -2866,19 +2903,19 @@
       </c>
       <c r="J33" s="22">
         <f t="shared" si="0"/>
-        <v>0.221</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="K33" s="22">
         <f t="shared" si="1"/>
-        <v>0.29899999999999999</v>
+        <v>0.28600000000000003</v>
       </c>
       <c r="L33" s="22">
         <f t="shared" si="2"/>
-        <v>0.18784999999999999</v>
+        <v>0.20800000000000002</v>
       </c>
       <c r="M33" s="22">
         <f t="shared" si="3"/>
-        <v>0.34384999999999993</v>
+        <v>0.312</v>
       </c>
       <c r="S33" s="14"/>
       <c r="T33" s="14"/>
@@ -2914,19 +2951,19 @@
       </c>
       <c r="J34" s="22">
         <f t="shared" si="0"/>
-        <v>0.22525000000000001</v>
+        <v>0.23850000000000002</v>
       </c>
       <c r="K34" s="22">
         <f t="shared" si="1"/>
-        <v>0.30474999999999997</v>
+        <v>0.29150000000000004</v>
       </c>
       <c r="L34" s="22">
         <f t="shared" si="2"/>
-        <v>0.19146250000000001</v>
+        <v>0.21200000000000002</v>
       </c>
       <c r="M34" s="22">
         <f t="shared" si="3"/>
-        <v>0.35046249999999995</v>
+        <v>0.318</v>
       </c>
       <c r="S34" s="14"/>
       <c r="T34" s="14"/>
@@ -2962,7 +2999,7 @@
       </c>
       <c r="J35" s="22">
         <f t="shared" si="0"/>
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="K35" s="22">
         <f t="shared" si="1"/>
@@ -2970,7 +3007,7 @@
       </c>
       <c r="L35" s="22">
         <f t="shared" si="2"/>
-        <v>0.72249999999999992</v>
+        <v>0.8</v>
       </c>
       <c r="M35" s="22">
         <f t="shared" si="3"/>
@@ -3010,19 +3047,19 @@
       </c>
       <c r="J36" s="22">
         <f t="shared" si="0"/>
-        <v>0.50149999999999995</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="K36" s="22">
         <f t="shared" si="1"/>
-        <v>0.67849999999999988</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="L36" s="22">
         <f t="shared" si="2"/>
-        <v>0.42627499999999996</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="M36" s="22">
         <f t="shared" si="3"/>
-        <v>0.78027499999999983</v>
+        <v>0.70799999999999996</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -3056,19 +3093,19 @@
       </c>
       <c r="J37" s="22">
         <f t="shared" si="0"/>
-        <v>0.255</v>
+        <v>0.27</v>
       </c>
       <c r="K37" s="22">
         <f t="shared" si="1"/>
-        <v>0.34499999999999997</v>
+        <v>0.33</v>
       </c>
       <c r="L37" s="22">
         <f t="shared" si="2"/>
-        <v>0.21675</v>
+        <v>0.24</v>
       </c>
       <c r="M37" s="22">
         <f t="shared" si="3"/>
-        <v>0.39674999999999994</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
@@ -3102,19 +3139,19 @@
       </c>
       <c r="J38" s="22">
         <f t="shared" si="0"/>
-        <v>0.17849999999999999</v>
+        <v>0.189</v>
       </c>
       <c r="K38" s="22">
         <f t="shared" si="1"/>
-        <v>0.24149999999999996</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="L38" s="22">
         <f t="shared" si="2"/>
-        <v>0.151725</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="M38" s="22">
         <f t="shared" si="3"/>
-        <v>0.27772499999999994</v>
+        <v>0.252</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
@@ -3148,19 +3185,19 @@
       </c>
       <c r="J39" s="22">
         <f t="shared" si="0"/>
-        <v>0.1615</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="K39" s="22">
         <f t="shared" si="1"/>
-        <v>0.21849999999999997</v>
+        <v>0.20900000000000002</v>
       </c>
       <c r="L39" s="22">
         <f t="shared" si="2"/>
-        <v>0.13727500000000001</v>
+        <v>0.15200000000000002</v>
       </c>
       <c r="M39" s="22">
         <f t="shared" si="3"/>
-        <v>0.25127499999999997</v>
+        <v>0.22799999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
@@ -3194,19 +3231,19 @@
       </c>
       <c r="J40" s="22">
         <f t="shared" si="0"/>
-        <v>0.14450000000000002</v>
+        <v>0.15300000000000002</v>
       </c>
       <c r="K40" s="22">
         <f t="shared" si="1"/>
-        <v>0.19550000000000001</v>
+        <v>0.18700000000000003</v>
       </c>
       <c r="L40" s="22">
         <f t="shared" si="2"/>
-        <v>0.12282500000000002</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="M40" s="22">
         <f t="shared" si="3"/>
-        <v>0.224825</v>
+        <v>0.20400000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
@@ -3240,19 +3277,19 @@
       </c>
       <c r="J41" s="22">
         <f t="shared" si="0"/>
-        <v>0.13175000000000001</v>
+        <v>0.13950000000000001</v>
       </c>
       <c r="K41" s="22">
         <f t="shared" si="1"/>
-        <v>0.17824999999999999</v>
+        <v>0.17050000000000001</v>
       </c>
       <c r="L41" s="22">
         <f t="shared" si="2"/>
-        <v>0.1119875</v>
+        <v>0.124</v>
       </c>
       <c r="M41" s="22">
         <f t="shared" si="3"/>
-        <v>0.20498749999999996</v>
+        <v>0.186</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -3286,19 +3323,19 @@
       </c>
       <c r="J42" s="22">
         <f t="shared" si="0"/>
-        <v>0.12324999999999998</v>
+        <v>0.1305</v>
       </c>
       <c r="K42" s="22">
         <f t="shared" si="1"/>
-        <v>0.16674999999999998</v>
+        <v>0.1595</v>
       </c>
       <c r="L42" s="22">
         <f t="shared" si="2"/>
-        <v>0.10476249999999998</v>
+        <v>0.11599999999999999</v>
       </c>
       <c r="M42" s="22">
         <f t="shared" si="3"/>
-        <v>0.19176249999999997</v>
+        <v>0.17399999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
@@ -3332,19 +3369,19 @@
       </c>
       <c r="J43" s="22">
         <f t="shared" si="0"/>
-        <v>0.1105</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="K43" s="22">
         <f t="shared" si="1"/>
-        <v>0.14949999999999999</v>
+        <v>0.14300000000000002</v>
       </c>
       <c r="L43" s="22">
         <f t="shared" si="2"/>
-        <v>9.3924999999999995E-2</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="M43" s="22">
         <f t="shared" si="3"/>
-        <v>0.17192499999999997</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
@@ -3378,19 +3415,19 @@
       </c>
       <c r="J44" s="22">
         <f t="shared" si="0"/>
-        <v>0.10199999999999999</v>
+        <v>0.108</v>
       </c>
       <c r="K44" s="22">
         <f t="shared" si="1"/>
-        <v>0.13799999999999998</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="L44" s="22">
         <f t="shared" si="2"/>
-        <v>8.6699999999999985E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="M44" s="22">
         <f t="shared" si="3"/>
-        <v>0.15869999999999998</v>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
@@ -3424,19 +3461,19 @@
       </c>
       <c r="J45" s="22">
         <f t="shared" si="0"/>
-        <v>8.5000000000000006E-2</v>
+        <v>9.0000000000000011E-2</v>
       </c>
       <c r="K45" s="22">
         <f t="shared" si="1"/>
-        <v>0.11499999999999999</v>
+        <v>0.11000000000000001</v>
       </c>
       <c r="L45" s="22">
         <f t="shared" si="2"/>
-        <v>7.2250000000000009E-2</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="M45" s="22">
         <f t="shared" si="3"/>
-        <v>0.13224999999999998</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
@@ -3470,18 +3507,18 @@
       </c>
       <c r="J47" s="22">
         <f t="shared" si="0"/>
-        <v>0.76500000000000001</v>
+        <v>0.81</v>
       </c>
       <c r="K47" s="22">
-        <f t="shared" ref="K47:K70" si="4">MIN(1, I47*1.15)</f>
-        <v>1</v>
+        <f t="shared" ref="K47:K70" si="4">MIN(1,I47*(1+$P$2))</f>
+        <v>0.9900000000000001</v>
       </c>
       <c r="L47" s="22">
-        <f t="shared" ref="L47:L70" si="5">MIN(1, J47*0.85)</f>
-        <v>0.65024999999999999</v>
+        <f t="shared" ref="L47:L70" si="5">MAX(0,I47*(1-$P$3))</f>
+        <v>0.72000000000000008</v>
       </c>
       <c r="M47" s="22">
-        <f t="shared" ref="M47:M70" si="6">MIN(1, K47*1.15)</f>
+        <f t="shared" ref="M47:M70" si="6">MIN(1,I47*(1+$P$3))</f>
         <v>1</v>
       </c>
     </row>
@@ -3516,7 +3553,7 @@
       </c>
       <c r="J48" s="22">
         <f t="shared" si="0"/>
-        <v>0.77349999999999997</v>
+        <v>0.81900000000000006</v>
       </c>
       <c r="K48" s="22">
         <f t="shared" si="4"/>
@@ -3524,7 +3561,7 @@
       </c>
       <c r="L48" s="22">
         <f t="shared" si="5"/>
-        <v>0.65747499999999992</v>
+        <v>0.72800000000000009</v>
       </c>
       <c r="M48" s="22">
         <f t="shared" si="6"/>
@@ -3562,7 +3599,7 @@
       </c>
       <c r="J49" s="22">
         <f t="shared" si="0"/>
-        <v>0.79049999999999998</v>
+        <v>0.83700000000000008</v>
       </c>
       <c r="K49" s="22">
         <f t="shared" si="4"/>
@@ -3570,7 +3607,7 @@
       </c>
       <c r="L49" s="22">
         <f t="shared" si="5"/>
-        <v>0.67192499999999999</v>
+        <v>0.74400000000000011</v>
       </c>
       <c r="M49" s="22">
         <f t="shared" si="6"/>
@@ -3608,7 +3645,7 @@
       </c>
       <c r="J50" s="22">
         <f t="shared" si="0"/>
-        <v>0.79049999999999998</v>
+        <v>0.83700000000000008</v>
       </c>
       <c r="K50" s="22">
         <f t="shared" si="4"/>
@@ -3616,7 +3653,7 @@
       </c>
       <c r="L50" s="22">
         <f t="shared" si="5"/>
-        <v>0.67192499999999999</v>
+        <v>0.74400000000000011</v>
       </c>
       <c r="M50" s="22">
         <f t="shared" si="6"/>
@@ -3654,7 +3691,7 @@
       </c>
       <c r="J51" s="22">
         <f t="shared" si="0"/>
-        <v>0.79899999999999993</v>
+        <v>0.84599999999999997</v>
       </c>
       <c r="K51" s="22">
         <f t="shared" si="4"/>
@@ -3662,7 +3699,7 @@
       </c>
       <c r="L51" s="22">
         <f t="shared" si="5"/>
-        <v>0.67914999999999992</v>
+        <v>0.752</v>
       </c>
       <c r="M51" s="22">
         <f t="shared" si="6"/>
@@ -3700,7 +3737,7 @@
       </c>
       <c r="J52" s="22">
         <f t="shared" si="0"/>
-        <v>0.8075</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="K52" s="22">
         <f t="shared" si="4"/>
@@ -3708,7 +3745,7 @@
       </c>
       <c r="L52" s="22">
         <f t="shared" si="5"/>
-        <v>0.68637499999999996</v>
+        <v>0.76</v>
       </c>
       <c r="M52" s="22">
         <f t="shared" si="6"/>
@@ -3746,19 +3783,19 @@
       </c>
       <c r="J53" s="22">
         <f t="shared" si="0"/>
-        <v>0.55249999999999999</v>
+        <v>0.58500000000000008</v>
       </c>
       <c r="K53" s="22">
         <f t="shared" si="4"/>
-        <v>0.74749999999999994</v>
+        <v>0.71500000000000008</v>
       </c>
       <c r="L53" s="22">
         <f t="shared" si="5"/>
-        <v>0.46962499999999996</v>
+        <v>0.52</v>
       </c>
       <c r="M53" s="22">
         <f t="shared" si="6"/>
-        <v>0.85962499999999986</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
@@ -3792,19 +3829,19 @@
       </c>
       <c r="J54" s="22">
         <f t="shared" si="0"/>
-        <v>0.60349999999999993</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="K54" s="22">
         <f t="shared" si="4"/>
-        <v>0.81649999999999989</v>
+        <v>0.78100000000000003</v>
       </c>
       <c r="L54" s="22">
         <f t="shared" si="5"/>
-        <v>0.51297499999999996</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="M54" s="22">
         <f t="shared" si="6"/>
-        <v>0.93897499999999978</v>
+        <v>0.85199999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -3838,19 +3875,19 @@
       </c>
       <c r="J55" s="22">
         <f t="shared" si="0"/>
-        <v>0.64600000000000002</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="K55" s="22">
         <f t="shared" si="4"/>
-        <v>0.87399999999999989</v>
+        <v>0.83600000000000008</v>
       </c>
       <c r="L55" s="22">
         <f t="shared" si="5"/>
-        <v>0.54910000000000003</v>
+        <v>0.6080000000000001</v>
       </c>
       <c r="M55" s="22">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.91199999999999992</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
@@ -3884,19 +3921,19 @@
       </c>
       <c r="J56" s="22">
         <f t="shared" si="0"/>
-        <v>0.67149999999999999</v>
+        <v>0.71100000000000008</v>
       </c>
       <c r="K56" s="22">
         <f t="shared" si="4"/>
-        <v>0.90849999999999997</v>
+        <v>0.86900000000000011</v>
       </c>
       <c r="L56" s="22">
         <f t="shared" si="5"/>
-        <v>0.57077499999999992</v>
+        <v>0.63200000000000012</v>
       </c>
       <c r="M56" s="22">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.94799999999999995</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
@@ -3930,19 +3967,19 @@
       </c>
       <c r="J57" s="22">
         <f t="shared" si="0"/>
-        <v>0.69699999999999995</v>
+        <v>0.73799999999999999</v>
       </c>
       <c r="K57" s="22">
         <f t="shared" si="4"/>
-        <v>0.94299999999999984</v>
+        <v>0.90200000000000002</v>
       </c>
       <c r="L57" s="22">
         <f t="shared" si="5"/>
-        <v>0.59244999999999992</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="M57" s="22">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.98399999999999987</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -3976,15 +4013,15 @@
       </c>
       <c r="J58" s="22">
         <f t="shared" si="0"/>
-        <v>0.72249999999999992</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="K58" s="22">
         <f t="shared" si="4"/>
-        <v>0.97749999999999992</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="L58" s="22">
         <f t="shared" si="5"/>
-        <v>0.61412499999999992</v>
+        <v>0.68</v>
       </c>
       <c r="M58" s="22">
         <f t="shared" si="6"/>
@@ -4022,19 +4059,19 @@
       </c>
       <c r="J59" s="22">
         <f t="shared" si="0"/>
-        <v>0.28900000000000003</v>
+        <v>0.30600000000000005</v>
       </c>
       <c r="K59" s="22">
         <f t="shared" si="4"/>
-        <v>0.39100000000000001</v>
+        <v>0.37400000000000005</v>
       </c>
       <c r="L59" s="22">
         <f t="shared" si="5"/>
-        <v>0.24565000000000003</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="M59" s="22">
         <f t="shared" si="6"/>
-        <v>0.44964999999999999</v>
+        <v>0.40800000000000003</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
@@ -4068,19 +4105,19 @@
       </c>
       <c r="J60" s="22">
         <f t="shared" si="0"/>
-        <v>0.32300000000000001</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="K60" s="22">
         <f t="shared" si="4"/>
-        <v>0.43699999999999994</v>
+        <v>0.41800000000000004</v>
       </c>
       <c r="L60" s="22">
         <f t="shared" si="5"/>
-        <v>0.27455000000000002</v>
+        <v>0.30400000000000005</v>
       </c>
       <c r="M60" s="22">
         <f t="shared" si="6"/>
-        <v>0.50254999999999994</v>
+        <v>0.45599999999999996</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
@@ -4114,19 +4151,19 @@
       </c>
       <c r="J61" s="22">
         <f t="shared" si="0"/>
-        <v>0.374</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="K61" s="22">
         <f t="shared" si="4"/>
-        <v>0.50600000000000001</v>
+        <v>0.48400000000000004</v>
       </c>
       <c r="L61" s="22">
         <f t="shared" si="5"/>
-        <v>0.31790000000000002</v>
+        <v>0.35200000000000004</v>
       </c>
       <c r="M61" s="22">
         <f t="shared" si="6"/>
-        <v>0.58189999999999997</v>
+        <v>0.52800000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
@@ -4160,19 +4197,19 @@
       </c>
       <c r="J62" s="22">
         <f t="shared" si="0"/>
-        <v>0.4335</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="K62" s="22">
         <f t="shared" si="4"/>
-        <v>0.58649999999999991</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="L62" s="22">
         <f t="shared" si="5"/>
-        <v>0.368475</v>
+        <v>0.40800000000000003</v>
       </c>
       <c r="M62" s="22">
         <f t="shared" si="6"/>
-        <v>0.67447499999999982</v>
+        <v>0.61199999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -4206,19 +4243,19 @@
       </c>
       <c r="J63" s="22">
         <f t="shared" si="0"/>
-        <v>0.48449999999999993</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="K63" s="22">
         <f t="shared" si="4"/>
-        <v>0.65549999999999986</v>
+        <v>0.627</v>
       </c>
       <c r="L63" s="22">
         <f t="shared" si="5"/>
-        <v>0.41182499999999994</v>
+        <v>0.45599999999999996</v>
       </c>
       <c r="M63" s="22">
         <f t="shared" si="6"/>
-        <v>0.75382499999999975</v>
+        <v>0.68399999999999994</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
@@ -4252,19 +4289,19 @@
       </c>
       <c r="J64" s="22">
         <f t="shared" si="0"/>
-        <v>0.55249999999999999</v>
+        <v>0.58500000000000008</v>
       </c>
       <c r="K64" s="22">
         <f t="shared" si="4"/>
-        <v>0.74749999999999994</v>
+        <v>0.71500000000000008</v>
       </c>
       <c r="L64" s="22">
         <f t="shared" si="5"/>
-        <v>0.46962499999999996</v>
+        <v>0.52</v>
       </c>
       <c r="M64" s="22">
         <f t="shared" si="6"/>
-        <v>0.85962499999999986</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
@@ -4298,19 +4335,19 @@
       </c>
       <c r="J65" s="22">
         <f t="shared" si="0"/>
-        <v>0.14450000000000002</v>
+        <v>0.15300000000000002</v>
       </c>
       <c r="K65" s="22">
         <f t="shared" si="4"/>
-        <v>0.19550000000000001</v>
+        <v>0.18700000000000003</v>
       </c>
       <c r="L65" s="22">
         <f t="shared" si="5"/>
-        <v>0.12282500000000002</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="M65" s="22">
         <f t="shared" si="6"/>
-        <v>0.224825</v>
+        <v>0.20400000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
@@ -4344,19 +4381,19 @@
       </c>
       <c r="J66" s="22">
         <f t="shared" si="0"/>
-        <v>0.20399999999999999</v>
+        <v>0.216</v>
       </c>
       <c r="K66" s="22">
         <f t="shared" si="4"/>
-        <v>0.27599999999999997</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="L66" s="22">
         <f t="shared" si="5"/>
-        <v>0.17339999999999997</v>
+        <v>0.192</v>
       </c>
       <c r="M66" s="22">
         <f t="shared" si="6"/>
-        <v>0.31739999999999996</v>
+        <v>0.28799999999999998</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
@@ -4389,20 +4426,20 @@
         <v>0.3</v>
       </c>
       <c r="J67" s="22">
-        <f t="shared" ref="J67:J70" si="7">MIN(1, I67*0.85)</f>
-        <v>0.255</v>
+        <f t="shared" ref="J67:J70" si="7">MAX(0,I67*(1-$P$2))</f>
+        <v>0.27</v>
       </c>
       <c r="K67" s="22">
         <f t="shared" si="4"/>
-        <v>0.34499999999999997</v>
+        <v>0.33</v>
       </c>
       <c r="L67" s="22">
         <f t="shared" si="5"/>
-        <v>0.21675</v>
+        <v>0.24</v>
       </c>
       <c r="M67" s="22">
         <f t="shared" si="6"/>
-        <v>0.39674999999999994</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
@@ -4436,19 +4473,19 @@
       </c>
       <c r="J68" s="22">
         <f t="shared" si="7"/>
-        <v>0.30599999999999999</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="K68" s="22">
         <f t="shared" si="4"/>
-        <v>0.41399999999999998</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="L68" s="22">
         <f t="shared" si="5"/>
-        <v>0.2601</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="M68" s="22">
         <f t="shared" si="6"/>
-        <v>0.47609999999999991</v>
+        <v>0.432</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
@@ -4482,19 +4519,19 @@
       </c>
       <c r="J69" s="22">
         <f t="shared" si="7"/>
-        <v>0.39949999999999997</v>
+        <v>0.42299999999999999</v>
       </c>
       <c r="K69" s="22">
         <f t="shared" si="4"/>
-        <v>0.54049999999999998</v>
+        <v>0.51700000000000002</v>
       </c>
       <c r="L69" s="22">
         <f t="shared" si="5"/>
-        <v>0.33957499999999996</v>
+        <v>0.376</v>
       </c>
       <c r="M69" s="22">
         <f t="shared" si="6"/>
-        <v>0.62157499999999988</v>
+        <v>0.56399999999999995</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
@@ -4528,19 +4565,19 @@
       </c>
       <c r="J70" s="22">
         <f t="shared" si="7"/>
-        <v>0.47600000000000003</v>
+        <v>0.50400000000000011</v>
       </c>
       <c r="K70" s="22">
         <f t="shared" si="4"/>
-        <v>0.64400000000000002</v>
+        <v>0.6160000000000001</v>
       </c>
       <c r="L70" s="22">
         <f t="shared" si="5"/>
-        <v>0.40460000000000002</v>
+        <v>0.44800000000000006</v>
       </c>
       <c r="M70" s="22">
         <f t="shared" si="6"/>
-        <v>0.74059999999999993</v>
+        <v>0.67200000000000004</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
@@ -4568,7 +4605,7 @@
         <v>55</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>43</v>
@@ -4586,9 +4623,11 @@
         <v>0.91980000000000006</v>
       </c>
       <c r="L72" s="22">
-        <v>0.67515000000000003</v>
+        <f t="shared" ref="L72:L119" si="8">MAX(0,I72*(1-$P$3))</f>
+        <v>0.72800000000000009</v>
       </c>
       <c r="M72" s="22">
+        <f t="shared" ref="M72:M119" si="9">MIN(1,I72*(1+$P$3))</f>
         <v>1</v>
       </c>
     </row>
@@ -4613,7 +4652,7 @@
         <v>55</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>43</v>
@@ -4631,9 +4670,11 @@
         <v>0.92980000000000007</v>
       </c>
       <c r="L73" s="22">
-        <v>0.68264999999999998</v>
+        <f t="shared" si="8"/>
+        <v>0.7360000000000001</v>
       </c>
       <c r="M73" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -4658,7 +4699,7 @@
         <v>55</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G74" s="13" t="s">
         <v>43</v>
@@ -4676,9 +4717,11 @@
         <v>0.93980000000000008</v>
       </c>
       <c r="L74" s="22">
-        <v>0.69015000000000004</v>
+        <f t="shared" si="8"/>
+        <v>0.74400000000000011</v>
       </c>
       <c r="M74" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -4703,7 +4746,7 @@
         <v>55</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>43</v>
@@ -4721,9 +4764,11 @@
         <v>0.94979999999999998</v>
       </c>
       <c r="L75" s="22">
-        <v>0.69764999999999988</v>
+        <f t="shared" si="8"/>
+        <v>0.752</v>
       </c>
       <c r="M75" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -4748,7 +4793,7 @@
         <v>55</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>43</v>
@@ -4766,9 +4811,11 @@
         <v>0.95979999999999999</v>
       </c>
       <c r="L76" s="22">
-        <v>0.70514999999999994</v>
+        <f t="shared" si="8"/>
+        <v>0.76</v>
       </c>
       <c r="M76" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -4793,7 +4840,7 @@
         <v>55</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>43</v>
@@ -4811,9 +4858,11 @@
         <v>0.97175999999999996</v>
       </c>
       <c r="L77" s="22">
-        <v>0.71117999999999992</v>
+        <f t="shared" si="8"/>
+        <v>0.76800000000000002</v>
       </c>
       <c r="M77" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -4838,7 +4887,7 @@
         <v>56</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>43</v>
@@ -4856,9 +4905,11 @@
         <v>0.86743999999999999</v>
       </c>
       <c r="L78" s="22">
-        <v>0.60941999999999996</v>
+        <f t="shared" si="8"/>
+        <v>0.67200000000000004</v>
       </c>
       <c r="M78" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -4883,7 +4934,7 @@
         <v>56</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>43</v>
@@ -4901,9 +4952,11 @@
         <v>0.9194</v>
       </c>
       <c r="L79" s="22">
-        <v>0.64545000000000008</v>
+        <f t="shared" si="8"/>
+        <v>0.71200000000000008</v>
       </c>
       <c r="M79" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -4928,7 +4981,7 @@
         <v>56</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G80" s="13" t="s">
         <v>43</v>
@@ -4946,9 +4999,11 @@
         <v>0.93332000000000004</v>
       </c>
       <c r="L80" s="22">
-        <v>0.65000999999999998</v>
+        <f t="shared" si="8"/>
+        <v>0.72000000000000008</v>
       </c>
       <c r="M80" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -4973,7 +5028,7 @@
         <v>56</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>43</v>
@@ -4991,9 +5046,11 @@
         <v>0.94724000000000008</v>
       </c>
       <c r="L81" s="22">
-        <v>0.65456999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.72800000000000009</v>
       </c>
       <c r="M81" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -5018,7 +5075,7 @@
         <v>56</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>43</v>
@@ -5036,9 +5093,11 @@
         <v>0.97116000000000002</v>
       </c>
       <c r="L82" s="22">
-        <v>0.66663000000000006</v>
+        <f t="shared" si="8"/>
+        <v>0.74400000000000011</v>
       </c>
       <c r="M82" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -5063,7 +5122,7 @@
         <v>56</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>43</v>
@@ -5081,9 +5140,11 @@
         <v>0.95900000000000007</v>
       </c>
       <c r="L83" s="22">
-        <v>0.64575000000000005</v>
+        <f t="shared" si="8"/>
+        <v>0.72800000000000009</v>
       </c>
       <c r="M83" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -5108,7 +5169,7 @@
         <v>57</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G84" s="14" t="s">
         <v>44</v>
@@ -5126,10 +5187,12 @@
         <v>0.76547999999999994</v>
       </c>
       <c r="L84" s="22">
-        <v>0.53588999999999998</v>
+        <f t="shared" si="8"/>
+        <v>0.59199999999999997</v>
       </c>
       <c r="M84" s="22">
-        <v>0.95684999999999998</v>
+        <f t="shared" si="9"/>
+        <v>0.88800000000000001</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
@@ -5153,7 +5216,7 @@
         <v>57</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G85" s="14" t="s">
         <v>44</v>
@@ -5171,10 +5234,12 @@
         <v>0.79744000000000004</v>
       </c>
       <c r="L85" s="22">
-        <v>0.55691999999999997</v>
+        <f t="shared" si="8"/>
+        <v>0.6160000000000001</v>
       </c>
       <c r="M85" s="22">
-        <v>0.99680000000000002</v>
+        <f t="shared" si="9"/>
+        <v>0.92399999999999993</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
@@ -5198,7 +5263,7 @@
         <v>57</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G86" s="14" t="s">
         <v>44</v>
@@ -5216,10 +5281,12 @@
         <v>0.82940000000000003</v>
       </c>
       <c r="L86" s="22">
-        <v>0.57795000000000007</v>
+        <f t="shared" si="8"/>
+        <v>0.64000000000000012</v>
       </c>
       <c r="M86" s="22">
-        <v>1</v>
+        <f t="shared" si="9"/>
+        <v>0.96</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
@@ -5243,7 +5310,7 @@
         <v>57</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G87" s="14" t="s">
         <v>44</v>
@@ -5261,10 +5328,12 @@
         <v>0.8613599999999999</v>
       </c>
       <c r="L87" s="22">
-        <v>0.59898000000000007</v>
+        <f t="shared" si="8"/>
+        <v>0.66400000000000003</v>
       </c>
       <c r="M87" s="22">
-        <v>1</v>
+        <f t="shared" si="9"/>
+        <v>0.99599999999999989</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
@@ -5288,7 +5357,7 @@
         <v>57</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G88" s="14" t="s">
         <v>44</v>
@@ -5306,9 +5375,11 @@
         <v>0.89332</v>
       </c>
       <c r="L88" s="22">
-        <v>0.62000999999999995</v>
+        <f t="shared" si="8"/>
+        <v>0.68800000000000006</v>
       </c>
       <c r="M88" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -5333,7 +5404,7 @@
         <v>57</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G89" s="14" t="s">
         <v>44</v>
@@ -5351,9 +5422,11 @@
         <v>0.91332000000000002</v>
       </c>
       <c r="L89" s="22">
-        <v>0.63500999999999996</v>
+        <f t="shared" si="8"/>
+        <v>0.70400000000000007</v>
       </c>
       <c r="M89" s="22">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -5375,10 +5448,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G90" s="14" t="s">
         <v>44</v>
@@ -5396,10 +5469,12 @@
         <v>0.53920000000000001</v>
       </c>
       <c r="L90" s="22">
-        <v>0.34560000000000002</v>
+        <f t="shared" si="8"/>
+        <v>0.4</v>
       </c>
       <c r="M90" s="22">
-        <v>0.67400000000000004</v>
+        <f t="shared" si="9"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
@@ -5420,10 +5495,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G91" s="14" t="s">
         <v>44</v>
@@ -5441,10 +5516,12 @@
         <v>0.65095999999999998</v>
       </c>
       <c r="L91" s="22">
-        <v>0.41177999999999998</v>
+        <f t="shared" si="8"/>
+        <v>0.48</v>
       </c>
       <c r="M91" s="22">
-        <v>0.81369999999999998</v>
+        <f t="shared" si="9"/>
+        <v>0.72</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
@@ -5465,10 +5542,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G92" s="14" t="s">
         <v>44</v>
@@ -5486,10 +5563,12 @@
         <v>0.71879999999999999</v>
       </c>
       <c r="L92" s="22">
-        <v>0.45090000000000008</v>
+        <f t="shared" si="8"/>
+        <v>0.52800000000000002</v>
       </c>
       <c r="M92" s="22">
-        <v>0.89849999999999997</v>
+        <f t="shared" si="9"/>
+        <v>0.79200000000000004</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
@@ -5510,10 +5589,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G93" s="14" t="s">
         <v>44</v>
@@ -5531,10 +5610,12 @@
         <v>0.76859999999999995</v>
       </c>
       <c r="L93" s="22">
-        <v>0.47354999999999997</v>
+        <f t="shared" si="8"/>
+        <v>0.55999999999999994</v>
       </c>
       <c r="M93" s="22">
-        <v>0.96074999999999999</v>
+        <f t="shared" si="9"/>
+        <v>0.84</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
@@ -5555,10 +5636,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G94" s="14" t="s">
         <v>44</v>
@@ -5576,10 +5657,12 @@
         <v>0.80035999999999996</v>
       </c>
       <c r="L94" s="22">
-        <v>0.47972999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.57599999999999996</v>
       </c>
       <c r="M94" s="22">
-        <v>1</v>
+        <f t="shared" si="9"/>
+        <v>0.86399999999999999</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
@@ -5600,10 +5683,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G95" s="14" t="s">
         <v>44</v>
@@ -5621,10 +5704,12 @@
         <v>0.85016000000000003</v>
       </c>
       <c r="L95" s="22">
-        <v>0.50238000000000005</v>
+        <f t="shared" si="8"/>
+        <v>0.6080000000000001</v>
       </c>
       <c r="M95" s="22">
-        <v>1</v>
+        <f t="shared" si="9"/>
+        <v>0.91199999999999992</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -5648,7 +5733,7 @@
         <v>58</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G96" s="14" t="s">
         <v>45</v>
@@ -5666,10 +5751,12 @@
         <v>0.44567999999999997</v>
       </c>
       <c r="L96" s="22">
-        <v>0.31074000000000002</v>
+        <f t="shared" si="8"/>
+        <v>0.34400000000000003</v>
       </c>
       <c r="M96" s="22">
-        <v>0.55709999999999993</v>
+        <f t="shared" si="9"/>
+        <v>0.51600000000000001</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
@@ -5693,7 +5780,7 @@
         <v>58</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G97" s="14" t="s">
         <v>45</v>
@@ -5711,10 +5798,12 @@
         <v>0.44763999999999998</v>
       </c>
       <c r="L97" s="22">
-        <v>0.30926999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.34400000000000003</v>
       </c>
       <c r="M97" s="22">
-        <v>0.55954999999999999</v>
+        <f t="shared" si="9"/>
+        <v>0.51600000000000001</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
@@ -5738,7 +5827,7 @@
         <v>58</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G98" s="14" t="s">
         <v>45</v>
@@ -5756,10 +5845,12 @@
         <v>0.49959999999999999</v>
       </c>
       <c r="L98" s="22">
-        <v>0.3453</v>
+        <f t="shared" si="8"/>
+        <v>0.38400000000000001</v>
       </c>
       <c r="M98" s="22">
-        <v>0.62449999999999994</v>
+        <f t="shared" si="9"/>
+        <v>0.57599999999999996</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
@@ -5783,7 +5874,7 @@
         <v>58</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G99" s="14" t="s">
         <v>45</v>
@@ -5801,10 +5892,12 @@
         <v>0.56547999999999998</v>
       </c>
       <c r="L99" s="22">
-        <v>0.38589000000000007</v>
+        <f t="shared" si="8"/>
+        <v>0.43200000000000005</v>
       </c>
       <c r="M99" s="22">
-        <v>0.70684999999999998</v>
+        <f t="shared" si="9"/>
+        <v>0.64800000000000002</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
@@ -5828,7 +5921,7 @@
         <v>58</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G100" s="14" t="s">
         <v>45</v>
@@ -5846,10 +5939,12 @@
         <v>0.62939999999999996</v>
       </c>
       <c r="L100" s="22">
-        <v>0.42795</v>
+        <f t="shared" si="8"/>
+        <v>0.48</v>
       </c>
       <c r="M100" s="22">
-        <v>0.78674999999999995</v>
+        <f t="shared" si="9"/>
+        <v>0.72</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
@@ -5873,7 +5968,7 @@
         <v>58</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G101" s="14" t="s">
         <v>45</v>
@@ -5891,10 +5986,12 @@
         <v>0.71332000000000007</v>
       </c>
       <c r="L101" s="22">
-        <v>0.48501000000000005</v>
+        <f t="shared" si="8"/>
+        <v>0.54400000000000004</v>
       </c>
       <c r="M101" s="22">
-        <v>0.89165000000000005</v>
+        <f t="shared" si="9"/>
+        <v>0.81600000000000006</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
@@ -5915,10 +6012,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F102" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G102" s="14" t="s">
         <v>45</v>
@@ -5936,10 +6033,12 @@
         <v>0.24372000000000002</v>
       </c>
       <c r="L102" s="22">
-        <v>0.16220999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.18400000000000002</v>
       </c>
       <c r="M102" s="22">
-        <v>0.30465000000000003</v>
+        <f t="shared" si="9"/>
+        <v>0.27600000000000002</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -5960,10 +6059,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F103" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G103" s="14" t="s">
         <v>45</v>
@@ -5981,10 +6080,12 @@
         <v>0.31156</v>
       </c>
       <c r="L103" s="22">
-        <v>0.20132999999999995</v>
+        <f t="shared" si="8"/>
+        <v>0.23199999999999998</v>
       </c>
       <c r="M103" s="22">
-        <v>0.38945000000000002</v>
+        <f t="shared" si="9"/>
+        <v>0.34799999999999998</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -6005,10 +6106,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F104" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G104" s="14" t="s">
         <v>45</v>
@@ -6026,10 +6127,12 @@
         <v>0.38939999999999997</v>
       </c>
       <c r="L104" s="22">
-        <v>0.24795</v>
+        <f t="shared" si="8"/>
+        <v>0.28799999999999998</v>
       </c>
       <c r="M104" s="22">
-        <v>0.48674999999999996</v>
+        <f t="shared" si="9"/>
+        <v>0.432</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
@@ -6050,10 +6153,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F105" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G105" s="14" t="s">
         <v>45</v>
@@ -6071,10 +6174,12 @@
         <v>0.4592</v>
       </c>
       <c r="L105" s="22">
-        <v>0.28559999999999997</v>
+        <f t="shared" si="8"/>
+        <v>0.33600000000000002</v>
       </c>
       <c r="M105" s="22">
-        <v>0.57399999999999995</v>
+        <f t="shared" si="9"/>
+        <v>0.504</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
@@ -6095,10 +6200,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E106" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F106" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G106" s="14" t="s">
         <v>45</v>
@@ -6116,10 +6221,12 @@
         <v>0.54096</v>
       </c>
       <c r="L106" s="22">
-        <v>0.32928000000000002</v>
+        <f t="shared" si="8"/>
+        <v>0.39200000000000002</v>
       </c>
       <c r="M106" s="22">
-        <v>0.67620000000000002</v>
+        <f t="shared" si="9"/>
+        <v>0.58799999999999997</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
@@ -6140,10 +6247,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E107" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F107" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G107" s="14" t="s">
         <v>45</v>
@@ -6161,10 +6268,12 @@
         <v>0.62860000000000005</v>
       </c>
       <c r="L107" s="22">
-        <v>0.36855000000000004</v>
+        <f t="shared" si="8"/>
+        <v>0.44800000000000006</v>
       </c>
       <c r="M107" s="22">
-        <v>0.78575000000000006</v>
+        <f t="shared" si="9"/>
+        <v>0.67200000000000004</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -6188,7 +6297,7 @@
         <v>59</v>
       </c>
       <c r="F108" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G108" s="14" t="s">
         <v>46</v>
@@ -6206,10 +6315,12 @@
         <v>0.24372000000000002</v>
       </c>
       <c r="L108" s="22">
-        <v>0.16220999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.18400000000000002</v>
       </c>
       <c r="M108" s="22">
-        <v>0.30465000000000003</v>
+        <f t="shared" si="9"/>
+        <v>0.27600000000000002</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
@@ -6233,7 +6344,7 @@
         <v>59</v>
       </c>
       <c r="F109" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G109" s="14" t="s">
         <v>46</v>
@@ -6251,10 +6362,12 @@
         <v>0.29764000000000002</v>
       </c>
       <c r="L109" s="22">
-        <v>0.19677000000000003</v>
+        <f t="shared" si="8"/>
+        <v>0.22400000000000003</v>
       </c>
       <c r="M109" s="22">
-        <v>0.37204999999999999</v>
+        <f t="shared" si="9"/>
+        <v>0.33600000000000002</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
@@ -6278,7 +6391,7 @@
         <v>59</v>
       </c>
       <c r="F110" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G110" s="14" t="s">
         <v>46</v>
@@ -6296,10 +6409,12 @@
         <v>0.36352000000000001</v>
       </c>
       <c r="L110" s="22">
-        <v>0.23736000000000002</v>
+        <f t="shared" si="8"/>
+        <v>0.27200000000000002</v>
       </c>
       <c r="M110" s="22">
-        <v>0.45440000000000003</v>
+        <f t="shared" si="9"/>
+        <v>0.40800000000000003</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
@@ -6323,7 +6438,7 @@
         <v>59</v>
       </c>
       <c r="F111" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G111" s="14" t="s">
         <v>46</v>
@@ -6341,10 +6456,12 @@
         <v>0.45135999999999998</v>
       </c>
       <c r="L111" s="22">
-        <v>0.29147999999999996</v>
+        <f t="shared" si="8"/>
+        <v>0.33600000000000002</v>
       </c>
       <c r="M111" s="22">
-        <v>0.56420000000000003</v>
+        <f t="shared" si="9"/>
+        <v>0.504</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
@@ -6368,7 +6485,7 @@
         <v>59</v>
       </c>
       <c r="F112" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G112" s="14" t="s">
         <v>46</v>
@@ -6386,10 +6503,12 @@
         <v>0.53723999999999994</v>
       </c>
       <c r="L112" s="22">
-        <v>0.34706999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.4</v>
       </c>
       <c r="M112" s="22">
-        <v>0.67154999999999987</v>
+        <f t="shared" si="9"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
@@ -6413,7 +6532,7 @@
         <v>59</v>
       </c>
       <c r="F113" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G113" s="14" t="s">
         <v>46</v>
@@ -6431,10 +6550,12 @@
         <v>0.63312000000000002</v>
       </c>
       <c r="L113" s="22">
-        <v>0.41015999999999997</v>
+        <f t="shared" si="8"/>
+        <v>0.47199999999999998</v>
       </c>
       <c r="M113" s="22">
-        <v>0.79139999999999999</v>
+        <f t="shared" si="9"/>
+        <v>0.70799999999999996</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
@@ -6455,10 +6576,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F114" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G114" s="14" t="s">
         <v>46</v>
@@ -6476,10 +6597,12 @@
         <v>0.1298</v>
       </c>
       <c r="L114" s="22">
-        <v>8.2650000000000001E-2</v>
+        <f t="shared" si="8"/>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="M114" s="22">
-        <v>0.16225000000000001</v>
+        <f t="shared" si="9"/>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
@@ -6500,10 +6623,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F115" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G115" s="14" t="s">
         <v>46</v>
@@ -6521,10 +6644,12 @@
         <v>0.19763999999999998</v>
       </c>
       <c r="L115" s="22">
-        <v>0.12177</v>
+        <f t="shared" si="8"/>
+        <v>0.14399999999999999</v>
       </c>
       <c r="M115" s="22">
-        <v>0.24704999999999999</v>
+        <f t="shared" si="9"/>
+        <v>0.216</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
@@ -6545,10 +6670,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F116" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G116" s="14" t="s">
         <v>46</v>
@@ -6566,10 +6691,12 @@
         <v>0.26744000000000001</v>
       </c>
       <c r="L116" s="22">
-        <v>0.15942000000000001</v>
+        <f t="shared" si="8"/>
+        <v>0.192</v>
       </c>
       <c r="M116" s="22">
-        <v>0.33430000000000004</v>
+        <f t="shared" si="9"/>
+        <v>0.28799999999999998</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
@@ -6590,10 +6717,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F117" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G117" s="14" t="s">
         <v>46</v>
@@ -6611,10 +6738,12 @@
         <v>0.35920000000000002</v>
       </c>
       <c r="L117" s="22">
-        <v>0.21060000000000001</v>
+        <f t="shared" si="8"/>
+        <v>0.25600000000000001</v>
       </c>
       <c r="M117" s="22">
-        <v>0.44900000000000001</v>
+        <f t="shared" si="9"/>
+        <v>0.38400000000000001</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.2">
@@ -6635,10 +6764,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E118" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F118" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G118" s="14" t="s">
         <v>46</v>
@@ -6656,10 +6785,12 @@
         <v>0.45292000000000004</v>
       </c>
       <c r="L118" s="22">
-        <v>0.26030999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.32000000000000006</v>
       </c>
       <c r="M118" s="22">
-        <v>0.56615000000000004</v>
+        <f t="shared" si="9"/>
+        <v>0.48</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.2">
@@ -6680,10 +6811,10 @@
         <v>Overall survival</v>
       </c>
       <c r="E119" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F119" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G119" s="14" t="s">
         <v>46</v>
@@ -6701,10 +6832,12 @@
         <v>0.56252000000000002</v>
       </c>
       <c r="L119" s="22">
-        <v>0.31311</v>
+        <f t="shared" si="8"/>
+        <v>0.39200000000000002</v>
       </c>
       <c r="M119" s="22">
-        <v>0.70315000000000005</v>
+        <f t="shared" si="9"/>
+        <v>0.58799999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More elegant selection of groups
And tweak to Best-Worst intervals on spreadsheet
</commit_message>
<xml_diff>
--- a/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
+++ b/ShinyApps/Conditional survival/data/ConditionalSurvival.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="plotsMetadata" sheetId="9" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="111">
   <si>
     <t>Ovarian cancer</t>
   </si>
@@ -263,12 +263,6 @@
   </si>
   <si>
     <t>p1</t>
-  </si>
-  <si>
-    <t>s1</t>
-  </si>
-  <si>
-    <t>s2</t>
   </si>
   <si>
     <t>datasetsID</t>
@@ -362,10 +356,19 @@
     <t>Ten-year (relative) overall survival curves in ovarian cancer by stage.</t>
   </si>
   <si>
-    <t>wbWidth</t>
-  </si>
-  <si>
     <t>ciWidth</t>
+  </si>
+  <si>
+    <t>inflation factor</t>
+  </si>
+  <si>
+    <t>time factoir</t>
+  </si>
+  <si>
+    <t>cs1</t>
+  </si>
+  <si>
+    <t>cs2</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -530,6 +533,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -814,9 +820,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,64 +850,64 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="H1" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="J1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="U1" s="6"/>
     </row>
@@ -929,7 +935,7 @@
         <v>53</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>49</v>
@@ -975,7 +981,7 @@
         <v>47</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>72</v>
@@ -1037,7 +1043,7 @@
         <v>47</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>74</v>
@@ -1047,7 +1053,7 @@
         <v>Ovarian cancer 5-yr conditional survival by age-group and stage (SEER 1988-2001)</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>39</v>
@@ -1302,9 +1308,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L74" sqref="L74"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1317,7 +1323,9 @@
     <col min="7" max="8" width="10.83203125" style="13"/>
     <col min="9" max="9" width="17.5" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="10.83203125" style="22"/>
-    <col min="14" max="16384" width="10.83203125" style="13"/>
+    <col min="14" max="14" width="10.83203125" style="13"/>
+    <col min="15" max="15" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -1338,31 +1346,31 @@
         <v>outcome</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>97</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>38</v>
       </c>
       <c r="I1" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="L1" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="M1" s="26" t="s">
         <v>100</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -1403,15 +1411,15 @@
         <v>1</v>
       </c>
       <c r="L2" s="22">
-        <f>MAX(0,I2*(1-$P$3))</f>
-        <v>0.8</v>
+        <f>MAX(0,I2-(I2-J2)*$P$3*($P$4 + H2)/(H2 + 1))</f>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M2" s="22">
-        <f>MIN(1,I2*(1+$P$3))</f>
+        <f>MIN(1, I2 + (I2-J2)*$P$3*($P$4 + H2)/(H2 + 1))</f>
         <v>1</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P2" s="32">
         <v>0.1</v>
@@ -1459,18 +1467,18 @@
         <v>1</v>
       </c>
       <c r="L3" s="22">
-        <f t="shared" ref="L3:L45" si="2">MAX(0,I3*(1-$P$3))</f>
-        <v>0.76800000000000002</v>
+        <f t="shared" ref="L3:L45" si="2">MAX(0,I3-(I3-J3)*$P$3*($P$4 + H3)/(H3 + 1))</f>
+        <v>0.67200000000000004</v>
       </c>
       <c r="M3" s="22">
-        <f t="shared" ref="M3:M45" si="3">MIN(1,I3*(1+$P$3))</f>
+        <f t="shared" ref="M3:M45" si="3">MIN(1, I3 + (I3-J3)*$P$3*($P$4 + H3)/(H3 + 1))</f>
         <v>1</v>
       </c>
       <c r="O3" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="P3" s="32">
-        <v>0.2</v>
+        <v>107</v>
+      </c>
+      <c r="P3" s="33">
+        <v>1.5</v>
       </c>
       <c r="S3" s="14"/>
       <c r="T3" s="14"/>
@@ -1514,11 +1522,17 @@
       </c>
       <c r="L4" s="22">
         <f t="shared" si="2"/>
-        <v>0.752</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="M4" s="22">
         <f t="shared" si="3"/>
         <v>1</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="P4" s="13">
+        <v>3</v>
       </c>
       <c r="S4" s="14"/>
       <c r="T4" s="14"/>
@@ -1562,7 +1576,7 @@
       </c>
       <c r="L5" s="22">
         <f t="shared" si="2"/>
-        <v>0.7360000000000001</v>
+        <v>0.71300000000000008</v>
       </c>
       <c r="M5" s="22">
         <f t="shared" si="3"/>
@@ -1610,7 +1624,7 @@
       </c>
       <c r="L6" s="22">
         <f t="shared" si="2"/>
-        <v>0.72000000000000008</v>
+        <v>0.71100000000000008</v>
       </c>
       <c r="M6" s="22">
         <f t="shared" si="3"/>
@@ -1706,7 +1720,7 @@
       </c>
       <c r="L8" s="22">
         <f t="shared" si="2"/>
-        <v>0.70400000000000007</v>
+        <v>0.71028571428571441</v>
       </c>
       <c r="M8" s="22">
         <f t="shared" si="3"/>
@@ -1754,7 +1768,7 @@
       </c>
       <c r="L9" s="22">
         <f t="shared" si="2"/>
-        <v>0.69600000000000006</v>
+        <v>0.70687500000000003</v>
       </c>
       <c r="M9" s="22">
         <f t="shared" si="3"/>
@@ -1802,7 +1816,7 @@
       </c>
       <c r="L10" s="22">
         <f t="shared" si="2"/>
-        <v>0.68800000000000006</v>
+        <v>0.70233333333333337</v>
       </c>
       <c r="M10" s="22">
         <f t="shared" si="3"/>
@@ -1850,7 +1864,7 @@
       </c>
       <c r="L11" s="22">
         <f t="shared" si="2"/>
-        <v>0.68400000000000005</v>
+        <v>0.70109999999999995</v>
       </c>
       <c r="M11" s="22">
         <f t="shared" si="3"/>
@@ -1898,7 +1912,7 @@
       </c>
       <c r="L12" s="22">
         <f t="shared" si="2"/>
-        <v>0.68</v>
+        <v>0.69931818181818184</v>
       </c>
       <c r="M12" s="22">
         <f t="shared" si="3"/>
@@ -1946,7 +1960,7 @@
       </c>
       <c r="L13" s="22">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M13" s="22">
         <f t="shared" si="3"/>
@@ -1999,7 +2013,7 @@
       </c>
       <c r="L14" s="22">
         <f t="shared" si="2"/>
-        <v>0.68800000000000006</v>
+        <v>0.60200000000000009</v>
       </c>
       <c r="M14" s="22">
         <f t="shared" si="3"/>
@@ -2047,11 +2061,11 @@
       </c>
       <c r="L15" s="22">
         <f t="shared" si="2"/>
-        <v>0.6080000000000001</v>
+        <v>0.57000000000000017</v>
       </c>
       <c r="M15" s="22">
         <f t="shared" si="3"/>
-        <v>0.91199999999999992</v>
+        <v>0.94999999999999984</v>
       </c>
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
@@ -2095,11 +2109,11 @@
       </c>
       <c r="L16" s="22">
         <f t="shared" si="2"/>
-        <v>0.58399999999999996</v>
+        <v>0.56575000000000009</v>
       </c>
       <c r="M16" s="22">
         <f t="shared" si="3"/>
-        <v>0.876</v>
+        <v>0.89424999999999988</v>
       </c>
       <c r="S16" s="14"/>
       <c r="T16" s="14"/>
@@ -2143,11 +2157,11 @@
       </c>
       <c r="L17" s="22">
         <f t="shared" si="2"/>
-        <v>0.55199999999999994</v>
+        <v>0.54510000000000003</v>
       </c>
       <c r="M17" s="22">
         <f t="shared" si="3"/>
-        <v>0.82799999999999996</v>
+        <v>0.83489999999999986</v>
       </c>
       <c r="S17" s="14"/>
       <c r="T17" s="14"/>
@@ -2191,11 +2205,11 @@
       </c>
       <c r="L18" s="22">
         <f t="shared" si="2"/>
-        <v>0.53600000000000003</v>
+        <v>0.53600000000000014</v>
       </c>
       <c r="M18" s="22">
         <f t="shared" si="3"/>
-        <v>0.80400000000000005</v>
+        <v>0.80399999999999994</v>
       </c>
       <c r="S18" s="14"/>
       <c r="T18" s="14"/>
@@ -2239,11 +2253,11 @@
       </c>
       <c r="L19" s="22">
         <f t="shared" si="2"/>
-        <v>0.52</v>
+        <v>0.5246428571428573</v>
       </c>
       <c r="M19" s="22">
         <f t="shared" si="3"/>
-        <v>0.78</v>
+        <v>0.77535714285714274</v>
       </c>
       <c r="S19" s="14"/>
       <c r="T19" s="14"/>
@@ -2287,11 +2301,11 @@
       </c>
       <c r="L20" s="22">
         <f t="shared" si="2"/>
-        <v>0.504</v>
+        <v>0.51187500000000008</v>
       </c>
       <c r="M20" s="22">
         <f t="shared" si="3"/>
-        <v>0.75600000000000001</v>
+        <v>0.74812499999999993</v>
       </c>
       <c r="S20" s="14"/>
       <c r="T20" s="14"/>
@@ -2335,11 +2349,11 @@
       </c>
       <c r="L21" s="22">
         <f t="shared" si="2"/>
-        <v>0.496</v>
+        <v>0.50633333333333341</v>
       </c>
       <c r="M21" s="22">
         <f t="shared" si="3"/>
-        <v>0.74399999999999999</v>
+        <v>0.73366666666666658</v>
       </c>
       <c r="S21" s="14"/>
       <c r="T21" s="14"/>
@@ -2383,11 +2397,11 @@
       </c>
       <c r="L22" s="22">
         <f t="shared" si="2"/>
-        <v>0.48799999999999999</v>
+        <v>0.50020000000000009</v>
       </c>
       <c r="M22" s="22">
         <f t="shared" si="3"/>
-        <v>0.73199999999999998</v>
+        <v>0.71979999999999988</v>
       </c>
       <c r="S22" s="14"/>
       <c r="T22" s="14"/>
@@ -2431,11 +2445,11 @@
       </c>
       <c r="L23" s="22">
         <f t="shared" si="2"/>
-        <v>0.48399999999999999</v>
+        <v>0.49775000000000003</v>
       </c>
       <c r="M23" s="22">
         <f t="shared" si="3"/>
-        <v>0.72599999999999998</v>
+        <v>0.71224999999999994</v>
       </c>
       <c r="S23" s="14"/>
       <c r="T23" s="14"/>
@@ -2479,7 +2493,7 @@
       </c>
       <c r="L24" s="22">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M24" s="22">
         <f t="shared" si="3"/>
@@ -2527,11 +2541,11 @@
       </c>
       <c r="L25" s="22">
         <f t="shared" si="2"/>
-        <v>0.6160000000000001</v>
+        <v>0.53900000000000015</v>
       </c>
       <c r="M25" s="22">
         <f t="shared" si="3"/>
-        <v>0.92399999999999993</v>
+        <v>1</v>
       </c>
       <c r="S25" s="14"/>
       <c r="T25" s="14"/>
@@ -2575,11 +2589,11 @@
       </c>
       <c r="L26" s="22">
         <f t="shared" si="2"/>
-        <v>0.504</v>
+        <v>0.47250000000000014</v>
       </c>
       <c r="M26" s="22">
         <f t="shared" si="3"/>
-        <v>0.75600000000000001</v>
+        <v>0.78749999999999987</v>
       </c>
       <c r="S26" s="14"/>
       <c r="T26" s="14"/>
@@ -2623,11 +2637,11 @@
       </c>
       <c r="L27" s="22">
         <f t="shared" si="2"/>
-        <v>0.40800000000000003</v>
+        <v>0.39525000000000005</v>
       </c>
       <c r="M27" s="22">
         <f t="shared" si="3"/>
-        <v>0.61199999999999999</v>
+        <v>0.62475000000000003</v>
       </c>
       <c r="S27" s="14"/>
       <c r="T27" s="14"/>
@@ -2671,11 +2685,11 @@
       </c>
       <c r="L28" s="22">
         <f t="shared" si="2"/>
-        <v>0.33600000000000002</v>
+        <v>0.33179999999999998</v>
       </c>
       <c r="M28" s="22">
         <f t="shared" si="3"/>
-        <v>0.504</v>
+        <v>0.50819999999999999</v>
       </c>
       <c r="S28" s="14"/>
       <c r="T28" s="14"/>
@@ -2719,11 +2733,11 @@
       </c>
       <c r="L29" s="22">
         <f t="shared" si="2"/>
-        <v>0.26400000000000001</v>
+        <v>0.26400000000000007</v>
       </c>
       <c r="M29" s="22">
         <f t="shared" si="3"/>
-        <v>0.39600000000000002</v>
+        <v>0.39599999999999996</v>
       </c>
       <c r="S29" s="14"/>
       <c r="T29" s="14"/>
@@ -2767,11 +2781,11 @@
       </c>
       <c r="L30" s="22">
         <f t="shared" si="2"/>
-        <v>0.24</v>
+        <v>0.24214285714285719</v>
       </c>
       <c r="M30" s="22">
         <f t="shared" si="3"/>
-        <v>0.36</v>
+        <v>0.35785714285714276</v>
       </c>
       <c r="S30" s="14"/>
       <c r="T30" s="14"/>
@@ -2815,11 +2829,11 @@
       </c>
       <c r="L31" s="22">
         <f t="shared" si="2"/>
-        <v>0.23199999999999998</v>
+        <v>0.23562500000000003</v>
       </c>
       <c r="M31" s="22">
         <f t="shared" si="3"/>
-        <v>0.34799999999999998</v>
+        <v>0.34437499999999993</v>
       </c>
       <c r="S31" s="14"/>
       <c r="T31" s="14"/>
@@ -2863,11 +2877,11 @@
       </c>
       <c r="L32" s="22">
         <f t="shared" si="2"/>
-        <v>0.21600000000000003</v>
+        <v>0.22050000000000003</v>
       </c>
       <c r="M32" s="22">
         <f t="shared" si="3"/>
-        <v>0.32400000000000001</v>
+        <v>0.31950000000000001</v>
       </c>
       <c r="S32" s="14"/>
       <c r="T32" s="14"/>
@@ -2911,11 +2925,11 @@
       </c>
       <c r="L33" s="22">
         <f t="shared" si="2"/>
-        <v>0.20800000000000002</v>
+        <v>0.2132</v>
       </c>
       <c r="M33" s="22">
         <f t="shared" si="3"/>
-        <v>0.312</v>
+        <v>0.30680000000000002</v>
       </c>
       <c r="S33" s="14"/>
       <c r="T33" s="14"/>
@@ -2959,11 +2973,11 @@
       </c>
       <c r="L34" s="22">
         <f t="shared" si="2"/>
-        <v>0.21200000000000002</v>
+        <v>0.21802272727272728</v>
       </c>
       <c r="M34" s="22">
         <f t="shared" si="3"/>
-        <v>0.318</v>
+        <v>0.31197727272727271</v>
       </c>
       <c r="S34" s="14"/>
       <c r="T34" s="14"/>
@@ -3007,7 +3021,7 @@
       </c>
       <c r="L35" s="22">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M35" s="22">
         <f t="shared" si="3"/>
@@ -3055,11 +3069,11 @@
       </c>
       <c r="L36" s="22">
         <f t="shared" si="2"/>
-        <v>0.47199999999999998</v>
+        <v>0.41300000000000014</v>
       </c>
       <c r="M36" s="22">
         <f t="shared" si="3"/>
-        <v>0.70799999999999996</v>
+        <v>0.76699999999999979</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -3101,11 +3115,11 @@
       </c>
       <c r="L37" s="22">
         <f t="shared" si="2"/>
-        <v>0.24</v>
+        <v>0.22500000000000006</v>
       </c>
       <c r="M37" s="22">
         <f t="shared" si="3"/>
-        <v>0.36</v>
+        <v>0.37499999999999989</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
@@ -3147,11 +3161,11 @@
       </c>
       <c r="L38" s="22">
         <f t="shared" si="2"/>
-        <v>0.16800000000000001</v>
+        <v>0.16275000000000001</v>
       </c>
       <c r="M38" s="22">
         <f t="shared" si="3"/>
-        <v>0.252</v>
+        <v>0.25724999999999998</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
@@ -3193,11 +3207,11 @@
       </c>
       <c r="L39" s="22">
         <f t="shared" si="2"/>
-        <v>0.15200000000000002</v>
+        <v>0.15010000000000001</v>
       </c>
       <c r="M39" s="22">
         <f t="shared" si="3"/>
-        <v>0.22799999999999998</v>
+        <v>0.22989999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
@@ -3239,11 +3253,11 @@
       </c>
       <c r="L40" s="22">
         <f t="shared" si="2"/>
-        <v>0.13600000000000001</v>
+        <v>0.13600000000000004</v>
       </c>
       <c r="M40" s="22">
         <f t="shared" si="3"/>
-        <v>0.20400000000000001</v>
+        <v>0.20399999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
@@ -3285,11 +3299,11 @@
       </c>
       <c r="L41" s="22">
         <f t="shared" si="2"/>
-        <v>0.124</v>
+        <v>0.12510714285714289</v>
       </c>
       <c r="M41" s="22">
         <f t="shared" si="3"/>
-        <v>0.186</v>
+        <v>0.18489285714285711</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -3331,11 +3345,11 @@
       </c>
       <c r="L42" s="22">
         <f t="shared" si="2"/>
-        <v>0.11599999999999999</v>
+        <v>0.11781250000000001</v>
       </c>
       <c r="M42" s="22">
         <f t="shared" si="3"/>
-        <v>0.17399999999999999</v>
+        <v>0.17218749999999997</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
@@ -3377,11 +3391,11 @@
       </c>
       <c r="L43" s="22">
         <f t="shared" si="2"/>
-        <v>0.10400000000000001</v>
+        <v>0.10616666666666667</v>
       </c>
       <c r="M43" s="22">
         <f t="shared" si="3"/>
-        <v>0.156</v>
+        <v>0.15383333333333332</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
@@ -3423,11 +3437,11 @@
       </c>
       <c r="L44" s="22">
         <f t="shared" si="2"/>
-        <v>9.6000000000000002E-2</v>
+        <v>9.8400000000000001E-2</v>
       </c>
       <c r="M44" s="22">
         <f t="shared" si="3"/>
-        <v>0.14399999999999999</v>
+        <v>0.1416</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
@@ -3469,11 +3483,11 @@
       </c>
       <c r="L45" s="22">
         <f t="shared" si="2"/>
-        <v>8.0000000000000016E-2</v>
+        <v>8.2272727272727289E-2</v>
       </c>
       <c r="M45" s="22">
         <f t="shared" si="3"/>
-        <v>0.12</v>
+        <v>0.11772727272727272</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
@@ -3490,8 +3504,8 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D47" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>43</v>
@@ -3514,11 +3528,11 @@
         <v>0.9900000000000001</v>
       </c>
       <c r="L47" s="22">
-        <f t="shared" ref="L47:L70" si="5">MAX(0,I47*(1-$P$3))</f>
-        <v>0.72000000000000008</v>
+        <f t="shared" ref="L47:L70" si="5">MAX(0,I47-(I47-J47)*$P$3)</f>
+        <v>0.76500000000000012</v>
       </c>
       <c r="M47" s="22">
-        <f t="shared" ref="M47:M70" si="6">MIN(1,I47*(1+$P$3))</f>
+        <f t="shared" ref="M47:M70" si="6">MIN(1, I47 + (I47 - J47)*$P$3)</f>
         <v>1</v>
       </c>
     </row>
@@ -3536,8 +3550,8 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D48" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>43</v>
@@ -3561,7 +3575,7 @@
       </c>
       <c r="L48" s="22">
         <f t="shared" si="5"/>
-        <v>0.72800000000000009</v>
+        <v>0.77350000000000008</v>
       </c>
       <c r="M48" s="22">
         <f t="shared" si="6"/>
@@ -3582,8 +3596,8 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D49" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>43</v>
@@ -3607,7 +3621,7 @@
       </c>
       <c r="L49" s="22">
         <f t="shared" si="5"/>
-        <v>0.74400000000000011</v>
+        <v>0.79050000000000009</v>
       </c>
       <c r="M49" s="22">
         <f t="shared" si="6"/>
@@ -3628,8 +3642,8 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D50" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>43</v>
@@ -3653,7 +3667,7 @@
       </c>
       <c r="L50" s="22">
         <f t="shared" si="5"/>
-        <v>0.74400000000000011</v>
+        <v>0.79050000000000009</v>
       </c>
       <c r="M50" s="22">
         <f t="shared" si="6"/>
@@ -3674,8 +3688,8 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D51" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E51" s="13" t="s">
         <v>43</v>
@@ -3699,7 +3713,7 @@
       </c>
       <c r="L51" s="22">
         <f t="shared" si="5"/>
-        <v>0.752</v>
+        <v>0.79899999999999993</v>
       </c>
       <c r="M51" s="22">
         <f t="shared" si="6"/>
@@ -3720,8 +3734,8 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D52" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E52" s="13" t="s">
         <v>43</v>
@@ -3745,7 +3759,7 @@
       </c>
       <c r="L52" s="22">
         <f t="shared" si="5"/>
-        <v>0.76</v>
+        <v>0.8075</v>
       </c>
       <c r="M52" s="22">
         <f t="shared" si="6"/>
@@ -3766,11 +3780,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D53" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>43</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="F53" s="14" t="s">
         <v>44</v>
@@ -3791,11 +3805,11 @@
       </c>
       <c r="L53" s="22">
         <f t="shared" si="5"/>
-        <v>0.52</v>
+        <v>0.5525000000000001</v>
       </c>
       <c r="M53" s="22">
         <f t="shared" si="6"/>
-        <v>0.78</v>
+        <v>0.74749999999999994</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
@@ -3812,11 +3826,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D54" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>43</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="F54" s="14" t="s">
         <v>44</v>
@@ -3837,11 +3851,11 @@
       </c>
       <c r="L54" s="22">
         <f t="shared" si="5"/>
-        <v>0.56799999999999995</v>
+        <v>0.60350000000000004</v>
       </c>
       <c r="M54" s="22">
         <f t="shared" si="6"/>
-        <v>0.85199999999999998</v>
+        <v>0.81649999999999989</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -3858,11 +3872,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D55" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
-      </c>
-      <c r="E55" s="13" t="s">
-        <v>43</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="F55" s="14" t="s">
         <v>44</v>
@@ -3883,11 +3897,11 @@
       </c>
       <c r="L55" s="22">
         <f t="shared" si="5"/>
-        <v>0.6080000000000001</v>
+        <v>0.64600000000000013</v>
       </c>
       <c r="M55" s="22">
         <f t="shared" si="6"/>
-        <v>0.91199999999999992</v>
+        <v>0.87399999999999989</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
@@ -3904,11 +3918,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D56" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
-      </c>
-      <c r="E56" s="13" t="s">
-        <v>43</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="F56" s="14" t="s">
         <v>44</v>
@@ -3929,11 +3943,11 @@
       </c>
       <c r="L56" s="22">
         <f t="shared" si="5"/>
-        <v>0.63200000000000012</v>
+        <v>0.6715000000000001</v>
       </c>
       <c r="M56" s="22">
         <f t="shared" si="6"/>
-        <v>0.94799999999999995</v>
+        <v>0.90849999999999997</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
@@ -3950,11 +3964,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D57" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
-      </c>
-      <c r="E57" s="13" t="s">
-        <v>43</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="F57" s="14" t="s">
         <v>44</v>
@@ -3975,11 +3989,11 @@
       </c>
       <c r="L57" s="22">
         <f t="shared" si="5"/>
-        <v>0.65600000000000003</v>
+        <v>0.69700000000000006</v>
       </c>
       <c r="M57" s="22">
         <f t="shared" si="6"/>
-        <v>0.98399999999999987</v>
+        <v>0.94299999999999984</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -3996,11 +4010,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D58" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>43</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="F58" s="14" t="s">
         <v>44</v>
@@ -4021,11 +4035,11 @@
       </c>
       <c r="L58" s="22">
         <f t="shared" si="5"/>
-        <v>0.68</v>
+        <v>0.72250000000000003</v>
       </c>
       <c r="M58" s="22">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.97749999999999992</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
@@ -4042,11 +4056,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D59" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F59" s="14" t="s">
         <v>45</v>
@@ -4067,11 +4081,11 @@
       </c>
       <c r="L59" s="22">
         <f t="shared" si="5"/>
-        <v>0.27200000000000002</v>
+        <v>0.28900000000000003</v>
       </c>
       <c r="M59" s="22">
         <f t="shared" si="6"/>
-        <v>0.40800000000000003</v>
+        <v>0.39100000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
@@ -4088,11 +4102,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D60" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E60" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F60" s="14" t="s">
         <v>45</v>
@@ -4113,11 +4127,11 @@
       </c>
       <c r="L60" s="22">
         <f t="shared" si="5"/>
-        <v>0.30400000000000005</v>
+        <v>0.32300000000000006</v>
       </c>
       <c r="M60" s="22">
         <f t="shared" si="6"/>
-        <v>0.45599999999999996</v>
+        <v>0.43699999999999994</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
@@ -4134,11 +4148,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D61" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F61" s="14" t="s">
         <v>45</v>
@@ -4159,11 +4173,11 @@
       </c>
       <c r="L61" s="22">
         <f t="shared" si="5"/>
-        <v>0.35200000000000004</v>
+        <v>0.374</v>
       </c>
       <c r="M61" s="22">
         <f t="shared" si="6"/>
-        <v>0.52800000000000002</v>
+        <v>0.50600000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
@@ -4180,11 +4194,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D62" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F62" s="14" t="s">
         <v>45</v>
@@ -4205,11 +4219,11 @@
       </c>
       <c r="L62" s="22">
         <f t="shared" si="5"/>
-        <v>0.40800000000000003</v>
+        <v>0.4335</v>
       </c>
       <c r="M62" s="22">
         <f t="shared" si="6"/>
-        <v>0.61199999999999999</v>
+        <v>0.58650000000000002</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -4226,11 +4240,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D63" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F63" s="14" t="s">
         <v>45</v>
@@ -4251,11 +4265,11 @@
       </c>
       <c r="L63" s="22">
         <f t="shared" si="5"/>
-        <v>0.45599999999999996</v>
+        <v>0.48450000000000004</v>
       </c>
       <c r="M63" s="22">
         <f t="shared" si="6"/>
-        <v>0.68399999999999994</v>
+        <v>0.65549999999999986</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
@@ -4272,11 +4286,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D64" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F64" s="14" t="s">
         <v>45</v>
@@ -4297,11 +4311,11 @@
       </c>
       <c r="L64" s="22">
         <f t="shared" si="5"/>
-        <v>0.52</v>
+        <v>0.5525000000000001</v>
       </c>
       <c r="M64" s="22">
         <f t="shared" si="6"/>
-        <v>0.78</v>
+        <v>0.74749999999999994</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
@@ -4318,11 +4332,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D65" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F65" s="14" t="s">
         <v>46</v>
@@ -4343,11 +4357,11 @@
       </c>
       <c r="L65" s="22">
         <f t="shared" si="5"/>
-        <v>0.13600000000000001</v>
+        <v>0.14450000000000002</v>
       </c>
       <c r="M65" s="22">
         <f t="shared" si="6"/>
-        <v>0.20400000000000001</v>
+        <v>0.19550000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
@@ -4364,11 +4378,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D66" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F66" s="14" t="s">
         <v>46</v>
@@ -4389,11 +4403,11 @@
       </c>
       <c r="L66" s="22">
         <f t="shared" si="5"/>
-        <v>0.192</v>
+        <v>0.20400000000000001</v>
       </c>
       <c r="M66" s="22">
         <f t="shared" si="6"/>
-        <v>0.28799999999999998</v>
+        <v>0.27599999999999997</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
@@ -4410,11 +4424,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D67" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F67" s="14" t="s">
         <v>46</v>
@@ -4435,11 +4449,11 @@
       </c>
       <c r="L67" s="22">
         <f t="shared" si="5"/>
-        <v>0.24</v>
+        <v>0.255</v>
       </c>
       <c r="M67" s="22">
         <f t="shared" si="6"/>
-        <v>0.36</v>
+        <v>0.34499999999999997</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
@@ -4456,11 +4470,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D68" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F68" s="14" t="s">
         <v>46</v>
@@ -4481,11 +4495,11 @@
       </c>
       <c r="L68" s="22">
         <f t="shared" si="5"/>
-        <v>0.28799999999999998</v>
+        <v>0.30600000000000005</v>
       </c>
       <c r="M68" s="22">
         <f t="shared" si="6"/>
-        <v>0.432</v>
+        <v>0.41399999999999992</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
@@ -4502,11 +4516,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D69" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F69" s="14" t="s">
         <v>46</v>
@@ -4527,11 +4541,11 @@
       </c>
       <c r="L69" s="22">
         <f t="shared" si="5"/>
-        <v>0.376</v>
+        <v>0.39949999999999997</v>
       </c>
       <c r="M69" s="22">
         <f t="shared" si="6"/>
-        <v>0.56399999999999995</v>
+        <v>0.54049999999999998</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
@@ -4548,11 +4562,11 @@
         <v>Ovarian cancer</v>
       </c>
       <c r="D70" s="13" t="str">
-        <f>plotsMetadata!$G$3</f>
-        <v>Conditional survival</v>
+        <f>plotsMetadata!$O$2</f>
+        <v>Overall survival</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F70" s="14" t="s">
         <v>46</v>
@@ -4573,11 +4587,11 @@
       </c>
       <c r="L70" s="22">
         <f t="shared" si="5"/>
-        <v>0.44800000000000006</v>
+        <v>0.47600000000000015</v>
       </c>
       <c r="M70" s="22">
         <f t="shared" si="6"/>
-        <v>0.67200000000000004</v>
+        <v>0.64399999999999991</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
@@ -4623,12 +4637,12 @@
         <v>0.91980000000000006</v>
       </c>
       <c r="L72" s="22">
-        <f t="shared" ref="L72:L119" si="8">MAX(0,I72*(1-$P$3))</f>
-        <v>0.72800000000000009</v>
+        <f t="shared" ref="L72:L119" si="8">MAX(0,I72-(I72-J72)*$P$3)</f>
+        <v>0.89529999999999998</v>
       </c>
       <c r="M72" s="22">
-        <f t="shared" ref="M72:M119" si="9">MIN(1,I72*(1+$P$3))</f>
-        <v>1</v>
+        <f t="shared" ref="M72:M119" si="9">MIN(1, I72 + (I72 - J72)*$P$3)</f>
+        <v>0.92470000000000008</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
@@ -4671,11 +4685,11 @@
       </c>
       <c r="L73" s="22">
         <f t="shared" si="8"/>
-        <v>0.7360000000000001</v>
+        <v>0.90529999999999999</v>
       </c>
       <c r="M73" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.93470000000000009</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
@@ -4718,11 +4732,11 @@
       </c>
       <c r="L74" s="22">
         <f t="shared" si="8"/>
-        <v>0.74400000000000011</v>
+        <v>0.9153</v>
       </c>
       <c r="M74" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.9447000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
@@ -4765,11 +4779,11 @@
       </c>
       <c r="L75" s="22">
         <f t="shared" si="8"/>
-        <v>0.752</v>
+        <v>0.9252999999999999</v>
       </c>
       <c r="M75" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.95469999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
@@ -4812,11 +4826,11 @@
       </c>
       <c r="L76" s="22">
         <f t="shared" si="8"/>
-        <v>0.76</v>
+        <v>0.93529999999999991</v>
       </c>
       <c r="M76" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.9647</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
@@ -4859,11 +4873,11 @@
       </c>
       <c r="L77" s="22">
         <f t="shared" si="8"/>
-        <v>0.76800000000000002</v>
+        <v>0.94235999999999998</v>
       </c>
       <c r="M77" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.97763999999999995</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
@@ -4906,11 +4920,11 @@
       </c>
       <c r="L78" s="22">
         <f t="shared" si="8"/>
-        <v>0.67200000000000004</v>
+        <v>0.79883999999999999</v>
       </c>
       <c r="M78" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.88115999999999994</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
@@ -4953,11 +4967,11 @@
       </c>
       <c r="L79" s="22">
         <f t="shared" si="8"/>
-        <v>0.71200000000000008</v>
+        <v>0.8459000000000001</v>
       </c>
       <c r="M79" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.93409999999999993</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
@@ -5000,11 +5014,11 @@
       </c>
       <c r="L80" s="22">
         <f t="shared" si="8"/>
-        <v>0.72000000000000008</v>
+        <v>0.85002</v>
       </c>
       <c r="M80" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.94998000000000005</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
@@ -5047,11 +5061,11 @@
       </c>
       <c r="L81" s="22">
         <f t="shared" si="8"/>
-        <v>0.72800000000000009</v>
+        <v>0.8541399999999999</v>
       </c>
       <c r="M81" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.96586000000000016</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
@@ -5094,11 +5108,11 @@
       </c>
       <c r="L82" s="22">
         <f t="shared" si="8"/>
-        <v>0.74400000000000011</v>
+        <v>0.86826000000000003</v>
       </c>
       <c r="M82" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.99174000000000007</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
@@ -5141,11 +5155,11 @@
       </c>
       <c r="L83" s="22">
         <f t="shared" si="8"/>
-        <v>0.72800000000000009</v>
+        <v>0.83650000000000002</v>
       </c>
       <c r="M83" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.98350000000000004</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
@@ -5188,11 +5202,11 @@
       </c>
       <c r="L84" s="22">
         <f t="shared" si="8"/>
-        <v>0.59199999999999997</v>
+        <v>0.70178000000000007</v>
       </c>
       <c r="M84" s="22">
         <f t="shared" si="9"/>
-        <v>0.88800000000000001</v>
+        <v>0.77821999999999991</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
@@ -5235,11 +5249,11 @@
       </c>
       <c r="L85" s="22">
         <f t="shared" si="8"/>
-        <v>0.6160000000000001</v>
+        <v>0.72883999999999993</v>
       </c>
       <c r="M85" s="22">
         <f t="shared" si="9"/>
-        <v>0.92399999999999993</v>
+        <v>0.8111600000000001</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
@@ -5282,11 +5296,11 @@
       </c>
       <c r="L86" s="22">
         <f t="shared" si="8"/>
-        <v>0.64000000000000012</v>
+        <v>0.75590000000000002</v>
       </c>
       <c r="M86" s="22">
         <f t="shared" si="9"/>
-        <v>0.96</v>
+        <v>0.84410000000000007</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
@@ -5329,11 +5343,11 @@
       </c>
       <c r="L87" s="22">
         <f t="shared" si="8"/>
-        <v>0.66400000000000003</v>
+        <v>0.7829600000000001</v>
       </c>
       <c r="M87" s="22">
         <f t="shared" si="9"/>
-        <v>0.99599999999999989</v>
+        <v>0.87703999999999982</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
@@ -5376,11 +5390,11 @@
       </c>
       <c r="L88" s="22">
         <f t="shared" si="8"/>
-        <v>0.68800000000000006</v>
+        <v>0.81001999999999996</v>
       </c>
       <c r="M88" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.90998000000000001</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
@@ -5423,11 +5437,11 @@
       </c>
       <c r="L89" s="22">
         <f t="shared" si="8"/>
-        <v>0.70400000000000007</v>
+        <v>0.83001999999999998</v>
       </c>
       <c r="M89" s="22">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.92998000000000003</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
@@ -5470,11 +5484,11 @@
       </c>
       <c r="L90" s="22">
         <f t="shared" si="8"/>
-        <v>0.4</v>
+        <v>0.44119999999999998</v>
       </c>
       <c r="M90" s="22">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.55879999999999996</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
@@ -5517,11 +5531,11 @@
       </c>
       <c r="L91" s="22">
         <f t="shared" si="8"/>
-        <v>0.48</v>
+        <v>0.52356000000000003</v>
       </c>
       <c r="M91" s="22">
         <f t="shared" si="9"/>
-        <v>0.72</v>
+        <v>0.67643999999999993</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
@@ -5564,11 +5578,11 @@
       </c>
       <c r="L92" s="22">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
+        <v>0.57180000000000009</v>
       </c>
       <c r="M92" s="22">
         <f t="shared" si="9"/>
-        <v>0.79200000000000004</v>
+        <v>0.74819999999999998</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
@@ -5611,11 +5625,11 @@
       </c>
       <c r="L93" s="22">
         <f t="shared" si="8"/>
-        <v>0.55999999999999994</v>
+        <v>0.59709999999999996</v>
       </c>
       <c r="M93" s="22">
         <f t="shared" si="9"/>
-        <v>0.84</v>
+        <v>0.80289999999999995</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
@@ -5658,11 +5672,11 @@
       </c>
       <c r="L94" s="22">
         <f t="shared" si="8"/>
-        <v>0.57599999999999996</v>
+        <v>0.59945999999999999</v>
       </c>
       <c r="M94" s="22">
         <f t="shared" si="9"/>
-        <v>0.86399999999999999</v>
+        <v>0.84053999999999995</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
@@ -5705,11 +5719,11 @@
       </c>
       <c r="L95" s="22">
         <f t="shared" si="8"/>
-        <v>0.6080000000000001</v>
+        <v>0.62475999999999998</v>
       </c>
       <c r="M95" s="22">
         <f t="shared" si="9"/>
-        <v>0.91199999999999992</v>
+        <v>0.89524000000000004</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -5752,11 +5766,11 @@
       </c>
       <c r="L96" s="22">
         <f t="shared" si="8"/>
-        <v>0.34400000000000003</v>
+        <v>0.40648000000000006</v>
       </c>
       <c r="M96" s="22">
         <f t="shared" si="9"/>
-        <v>0.51600000000000001</v>
+        <v>0.45351999999999992</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
@@ -5799,11 +5813,11 @@
       </c>
       <c r="L97" s="22">
         <f t="shared" si="8"/>
-        <v>0.34400000000000003</v>
+        <v>0.40354000000000001</v>
       </c>
       <c r="M97" s="22">
         <f t="shared" si="9"/>
-        <v>0.51600000000000001</v>
+        <v>0.45645999999999998</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
@@ -5846,11 +5860,11 @@
       </c>
       <c r="L98" s="22">
         <f t="shared" si="8"/>
-        <v>0.38400000000000001</v>
+        <v>0.4506</v>
       </c>
       <c r="M98" s="22">
         <f t="shared" si="9"/>
-        <v>0.57599999999999996</v>
+        <v>0.50939999999999996</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
@@ -5893,11 +5907,11 @@
       </c>
       <c r="L99" s="22">
         <f t="shared" si="8"/>
-        <v>0.43200000000000005</v>
+        <v>0.50178000000000011</v>
       </c>
       <c r="M99" s="22">
         <f t="shared" si="9"/>
-        <v>0.64800000000000002</v>
+        <v>0.57821999999999996</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
@@ -5940,11 +5954,11 @@
       </c>
       <c r="L100" s="22">
         <f t="shared" si="8"/>
-        <v>0.48</v>
+        <v>0.55590000000000006</v>
       </c>
       <c r="M100" s="22">
         <f t="shared" si="9"/>
-        <v>0.72</v>
+        <v>0.64409999999999989</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
@@ -5987,11 +6001,11 @@
       </c>
       <c r="L101" s="22">
         <f t="shared" si="8"/>
-        <v>0.54400000000000004</v>
+        <v>0.63002000000000002</v>
       </c>
       <c r="M101" s="22">
         <f t="shared" si="9"/>
-        <v>0.81600000000000006</v>
+        <v>0.72998000000000007</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
@@ -6034,11 +6048,11 @@
       </c>
       <c r="L102" s="22">
         <f t="shared" si="8"/>
-        <v>0.18400000000000002</v>
+        <v>0.20942</v>
       </c>
       <c r="M102" s="22">
         <f t="shared" si="9"/>
-        <v>0.27600000000000002</v>
+        <v>0.25058000000000002</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -6081,11 +6095,11 @@
       </c>
       <c r="L103" s="22">
         <f t="shared" si="8"/>
-        <v>0.23199999999999998</v>
+        <v>0.25765999999999994</v>
       </c>
       <c r="M103" s="22">
         <f t="shared" si="9"/>
-        <v>0.34799999999999998</v>
+        <v>0.32234000000000002</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
@@ -6128,11 +6142,11 @@
       </c>
       <c r="L104" s="22">
         <f t="shared" si="8"/>
-        <v>0.28799999999999998</v>
+        <v>0.31590000000000001</v>
       </c>
       <c r="M104" s="22">
         <f t="shared" si="9"/>
-        <v>0.432</v>
+        <v>0.40409999999999996</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
@@ -6175,11 +6189,11 @@
       </c>
       <c r="L105" s="22">
         <f t="shared" si="8"/>
-        <v>0.33600000000000002</v>
+        <v>0.36119999999999997</v>
       </c>
       <c r="M105" s="22">
         <f t="shared" si="9"/>
-        <v>0.504</v>
+        <v>0.4788</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
@@ -6222,11 +6236,11 @@
       </c>
       <c r="L106" s="22">
         <f t="shared" si="8"/>
-        <v>0.39200000000000002</v>
+        <v>0.41355999999999998</v>
       </c>
       <c r="M106" s="22">
         <f t="shared" si="9"/>
-        <v>0.58799999999999997</v>
+        <v>0.56644000000000005</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
@@ -6269,11 +6283,11 @@
       </c>
       <c r="L107" s="22">
         <f t="shared" si="8"/>
-        <v>0.44800000000000006</v>
+        <v>0.45710000000000006</v>
       </c>
       <c r="M107" s="22">
         <f t="shared" si="9"/>
-        <v>0.67200000000000004</v>
+        <v>0.66290000000000004</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -6316,11 +6330,11 @@
       </c>
       <c r="L108" s="22">
         <f t="shared" si="8"/>
-        <v>0.18400000000000002</v>
+        <v>0.20942</v>
       </c>
       <c r="M108" s="22">
         <f t="shared" si="9"/>
-        <v>0.27600000000000002</v>
+        <v>0.25058000000000002</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
@@ -6363,11 +6377,11 @@
       </c>
       <c r="L109" s="22">
         <f t="shared" si="8"/>
-        <v>0.22400000000000003</v>
+        <v>0.25354000000000004</v>
       </c>
       <c r="M109" s="22">
         <f t="shared" si="9"/>
-        <v>0.33600000000000002</v>
+        <v>0.30646000000000001</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
@@ -6410,11 +6424,11 @@
       </c>
       <c r="L110" s="22">
         <f t="shared" si="8"/>
-        <v>0.27200000000000002</v>
+        <v>0.30472000000000005</v>
       </c>
       <c r="M110" s="22">
         <f t="shared" si="9"/>
-        <v>0.40800000000000003</v>
+        <v>0.37528</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
@@ -6457,11 +6471,11 @@
       </c>
       <c r="L111" s="22">
         <f t="shared" si="8"/>
-        <v>0.33600000000000002</v>
+        <v>0.37295999999999996</v>
       </c>
       <c r="M111" s="22">
         <f t="shared" si="9"/>
-        <v>0.504</v>
+        <v>0.46704000000000001</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
@@ -6504,11 +6518,11 @@
       </c>
       <c r="L112" s="22">
         <f t="shared" si="8"/>
-        <v>0.4</v>
+        <v>0.44413999999999998</v>
       </c>
       <c r="M112" s="22">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.55586000000000002</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
@@ -6551,11 +6565,11 @@
       </c>
       <c r="L113" s="22">
         <f t="shared" si="8"/>
-        <v>0.47199999999999998</v>
+        <v>0.5253199999999999</v>
       </c>
       <c r="M113" s="22">
         <f t="shared" si="9"/>
-        <v>0.70799999999999996</v>
+        <v>0.65468000000000004</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
@@ -6598,11 +6612,11 @@
       </c>
       <c r="L114" s="22">
         <f t="shared" si="8"/>
-        <v>9.6000000000000002E-2</v>
+        <v>0.10529999999999999</v>
       </c>
       <c r="M114" s="22">
         <f t="shared" si="9"/>
-        <v>0.14399999999999999</v>
+        <v>0.13469999999999999</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
@@ -6645,11 +6659,11 @@
       </c>
       <c r="L115" s="22">
         <f t="shared" si="8"/>
-        <v>0.14399999999999999</v>
+        <v>0.15354000000000001</v>
       </c>
       <c r="M115" s="22">
         <f t="shared" si="9"/>
-        <v>0.216</v>
+        <v>0.20645999999999998</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
@@ -6692,11 +6706,11 @@
       </c>
       <c r="L116" s="22">
         <f t="shared" si="8"/>
-        <v>0.192</v>
+        <v>0.19884000000000002</v>
       </c>
       <c r="M116" s="22">
         <f t="shared" si="9"/>
-        <v>0.28799999999999998</v>
+        <v>0.28115999999999997</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
@@ -6739,11 +6753,11 @@
       </c>
       <c r="L117" s="22">
         <f t="shared" si="8"/>
-        <v>0.25600000000000001</v>
+        <v>0.26119999999999999</v>
       </c>
       <c r="M117" s="22">
         <f t="shared" si="9"/>
-        <v>0.38400000000000001</v>
+        <v>0.37880000000000003</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.2">
@@ -6786,11 +6800,11 @@
       </c>
       <c r="L118" s="22">
         <f t="shared" si="8"/>
-        <v>0.32000000000000006</v>
+        <v>0.32062000000000002</v>
       </c>
       <c r="M118" s="22">
         <f t="shared" si="9"/>
-        <v>0.48</v>
+        <v>0.47938000000000003</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.2">
@@ -6833,11 +6847,11 @@
       </c>
       <c r="L119" s="22">
         <f t="shared" si="8"/>
-        <v>0.39200000000000002</v>
+        <v>0.38121999999999995</v>
       </c>
       <c r="M119" s="22">
         <f t="shared" si="9"/>
-        <v>0.58799999999999997</v>
+        <v>0.59878000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>